<commit_message>
Fix several errors in reports 2-4 after review
</commit_message>
<xml_diff>
--- a/Practica 1. Mixturas de Gaussianas/resultados.xlsx
+++ b/Practica 1. Mixturas de Gaussianas/resultados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel\Nextcloud\ETSINF\2019-20\APR\Practicas\Practica 1. Mixturas de Gaussianas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{696B1D9F-E32F-488B-ABF0-2B3B808AF29B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8B3042-6E57-48E7-984B-CD6E74A0E1E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="27300" windowHeight="15960" activeTab="1" xr2:uid="{70A85A1C-AA30-458D-A4B6-11A0960EF6D5}"/>
   </bookViews>
@@ -160,7 +160,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -188,6 +188,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -219,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -228,12 +234,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -249,6 +249,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -13814,7 +13823,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{913AA4B1-433E-48F9-A0E5-825C8364C741}">
   <dimension ref="A1:H129"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="W29" sqref="W29"/>
     </sheetView>
   </sheetViews>
@@ -13824,22 +13833,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
       <c r="C2" s="2">
         <v>0.5</v>
       </c>
@@ -13860,7 +13869,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2">
@@ -13884,7 +13893,7 @@
       <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="2">
         <v>2</v>
       </c>
@@ -13906,7 +13915,7 @@
       <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="2">
         <v>3</v>
       </c>
@@ -13928,7 +13937,7 @@
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="2">
         <v>4</v>
       </c>
@@ -13950,7 +13959,7 @@
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="2">
         <v>5</v>
       </c>
@@ -13972,7 +13981,7 @@
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="2">
         <v>6</v>
       </c>
@@ -13994,7 +14003,7 @@
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="2">
         <v>7</v>
       </c>
@@ -14016,7 +14025,7 @@
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="2">
         <v>8</v>
       </c>
@@ -14038,7 +14047,7 @@
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="2">
         <v>9</v>
       </c>
@@ -14060,7 +14069,7 @@
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="2">
         <v>10</v>
       </c>
@@ -14082,22 +14091,22 @@
       <c r="H12" s="3"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="4" t="s">
+      <c r="B14" s="10"/>
+      <c r="C14" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
       <c r="C15" s="2">
         <v>0.5</v>
       </c>
@@ -14118,7 +14127,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B16" s="2">
@@ -14142,7 +14151,7 @@
       <c r="H16" s="3"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
+      <c r="A17" s="9"/>
       <c r="B17" s="2">
         <v>2</v>
       </c>
@@ -14164,7 +14173,7 @@
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
+      <c r="A18" s="9"/>
       <c r="B18" s="2">
         <v>3</v>
       </c>
@@ -14186,7 +14195,7 @@
       <c r="H18" s="3"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
+      <c r="A19" s="9"/>
       <c r="B19" s="2">
         <v>4</v>
       </c>
@@ -14208,7 +14217,7 @@
       <c r="H19" s="3"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
+      <c r="A20" s="9"/>
       <c r="B20" s="2">
         <v>5</v>
       </c>
@@ -14230,7 +14239,7 @@
       <c r="H20" s="3"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
+      <c r="A21" s="9"/>
       <c r="B21" s="2">
         <v>6</v>
       </c>
@@ -14252,7 +14261,7 @@
       <c r="H21" s="3"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
+      <c r="A22" s="9"/>
       <c r="B22" s="2">
         <v>7</v>
       </c>
@@ -14274,7 +14283,7 @@
       <c r="H22" s="3"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
+      <c r="A23" s="9"/>
       <c r="B23" s="2">
         <v>8</v>
       </c>
@@ -14296,7 +14305,7 @@
       <c r="H23" s="3"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
+      <c r="A24" s="9"/>
       <c r="B24" s="2">
         <v>9</v>
       </c>
@@ -14318,7 +14327,7 @@
       <c r="H24" s="3"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
+      <c r="A25" s="9"/>
       <c r="B25" s="2">
         <v>10</v>
       </c>
@@ -14340,22 +14349,22 @@
       <c r="H25" s="3"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="4" t="s">
+      <c r="B27" s="10"/>
+      <c r="C27" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
       <c r="C28" s="2">
         <v>0.5</v>
       </c>
@@ -14376,7 +14385,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B29" s="2">
@@ -14400,7 +14409,7 @@
       <c r="H29" s="3"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
+      <c r="A30" s="9"/>
       <c r="B30" s="2">
         <v>2</v>
       </c>
@@ -14422,7 +14431,7 @@
       <c r="H30" s="3"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
+      <c r="A31" s="9"/>
       <c r="B31" s="2">
         <v>3</v>
       </c>
@@ -14444,7 +14453,7 @@
       <c r="H31" s="3"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
+      <c r="A32" s="9"/>
       <c r="B32" s="2">
         <v>4</v>
       </c>
@@ -14466,7 +14475,7 @@
       <c r="H32" s="3"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
+      <c r="A33" s="9"/>
       <c r="B33" s="2">
         <v>5</v>
       </c>
@@ -14488,7 +14497,7 @@
       <c r="H33" s="3"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
+      <c r="A34" s="9"/>
       <c r="B34" s="2">
         <v>6</v>
       </c>
@@ -14510,7 +14519,7 @@
       <c r="H34" s="3"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
+      <c r="A35" s="9"/>
       <c r="B35" s="2">
         <v>7</v>
       </c>
@@ -14532,7 +14541,7 @@
       <c r="H35" s="3"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
+      <c r="A36" s="9"/>
       <c r="B36" s="2">
         <v>8</v>
       </c>
@@ -14554,7 +14563,7 @@
       <c r="H36" s="3"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
+      <c r="A37" s="9"/>
       <c r="B37" s="2">
         <v>9</v>
       </c>
@@ -14576,7 +14585,7 @@
       <c r="H37" s="3"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
+      <c r="A38" s="9"/>
       <c r="B38" s="2">
         <v>10</v>
       </c>
@@ -14598,22 +14607,22 @@
       <c r="H38" s="3"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
+      <c r="A40" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B40" s="5"/>
-      <c r="C40" s="4" t="s">
+      <c r="B40" s="10"/>
+      <c r="C40" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
+      <c r="A41" s="10"/>
+      <c r="B41" s="10"/>
       <c r="C41" s="2">
         <v>0.5</v>
       </c>
@@ -14634,7 +14643,7 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B42" s="2">
@@ -14658,7 +14667,7 @@
       <c r="H42" s="3"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="4"/>
+      <c r="A43" s="9"/>
       <c r="B43" s="2">
         <v>2</v>
       </c>
@@ -14680,7 +14689,7 @@
       <c r="H43" s="3"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
+      <c r="A44" s="9"/>
       <c r="B44" s="2">
         <v>3</v>
       </c>
@@ -14702,7 +14711,7 @@
       <c r="H44" s="3"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="4"/>
+      <c r="A45" s="9"/>
       <c r="B45" s="2">
         <v>4</v>
       </c>
@@ -14724,7 +14733,7 @@
       <c r="H45" s="3"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="4"/>
+      <c r="A46" s="9"/>
       <c r="B46" s="2">
         <v>5</v>
       </c>
@@ -14746,7 +14755,7 @@
       <c r="H46" s="3"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="4"/>
+      <c r="A47" s="9"/>
       <c r="B47" s="2">
         <v>6</v>
       </c>
@@ -14768,7 +14777,7 @@
       <c r="H47" s="3"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="4"/>
+      <c r="A48" s="9"/>
       <c r="B48" s="2">
         <v>7</v>
       </c>
@@ -14790,7 +14799,7 @@
       <c r="H48" s="3"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="4"/>
+      <c r="A49" s="9"/>
       <c r="B49" s="2">
         <v>8</v>
       </c>
@@ -14812,7 +14821,7 @@
       <c r="H49" s="3"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="4"/>
+      <c r="A50" s="9"/>
       <c r="B50" s="2">
         <v>9</v>
       </c>
@@ -14834,7 +14843,7 @@
       <c r="H50" s="3"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="4"/>
+      <c r="A51" s="9"/>
       <c r="B51" s="2">
         <v>10</v>
       </c>
@@ -14856,22 +14865,22 @@
       <c r="H51" s="3"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
+      <c r="A53" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B53" s="5"/>
-      <c r="C53" s="4" t="s">
+      <c r="B53" s="10"/>
+      <c r="C53" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="4"/>
-      <c r="G53" s="4"/>
-      <c r="H53" s="4"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="9"/>
+      <c r="H53" s="9"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="5"/>
-      <c r="B54" s="5"/>
+      <c r="A54" s="10"/>
+      <c r="B54" s="10"/>
       <c r="C54" s="2">
         <v>0.5</v>
       </c>
@@ -14892,7 +14901,7 @@
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
+      <c r="A55" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B55" s="2">
@@ -14916,7 +14925,7 @@
       <c r="H55" s="3"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="4"/>
+      <c r="A56" s="9"/>
       <c r="B56" s="2">
         <v>2</v>
       </c>
@@ -14938,7 +14947,7 @@
       <c r="H56" s="3"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="4"/>
+      <c r="A57" s="9"/>
       <c r="B57" s="2">
         <v>3</v>
       </c>
@@ -14960,7 +14969,7 @@
       <c r="H57" s="3"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="4"/>
+      <c r="A58" s="9"/>
       <c r="B58" s="2">
         <v>4</v>
       </c>
@@ -14982,7 +14991,7 @@
       <c r="H58" s="3"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="4"/>
+      <c r="A59" s="9"/>
       <c r="B59" s="2">
         <v>5</v>
       </c>
@@ -15004,7 +15013,7 @@
       <c r="H59" s="3"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="4"/>
+      <c r="A60" s="9"/>
       <c r="B60" s="2">
         <v>6</v>
       </c>
@@ -15026,7 +15035,7 @@
       <c r="H60" s="3"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="4"/>
+      <c r="A61" s="9"/>
       <c r="B61" s="2">
         <v>7</v>
       </c>
@@ -15048,7 +15057,7 @@
       <c r="H61" s="3"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="4"/>
+      <c r="A62" s="9"/>
       <c r="B62" s="2">
         <v>8</v>
       </c>
@@ -15070,7 +15079,7 @@
       <c r="H62" s="3"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="4"/>
+      <c r="A63" s="9"/>
       <c r="B63" s="2">
         <v>9</v>
       </c>
@@ -15092,7 +15101,7 @@
       <c r="H63" s="3"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="4"/>
+      <c r="A64" s="9"/>
       <c r="B64" s="2">
         <v>10</v>
       </c>
@@ -15114,22 +15123,22 @@
       <c r="H64" s="3"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="5" t="s">
+      <c r="A66" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B66" s="5"/>
-      <c r="C66" s="4" t="s">
+      <c r="B66" s="10"/>
+      <c r="C66" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D66" s="4"/>
-      <c r="E66" s="4"/>
-      <c r="F66" s="4"/>
-      <c r="G66" s="4"/>
-      <c r="H66" s="4"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="9"/>
+      <c r="F66" s="9"/>
+      <c r="G66" s="9"/>
+      <c r="H66" s="9"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="5"/>
-      <c r="B67" s="5"/>
+      <c r="A67" s="10"/>
+      <c r="B67" s="10"/>
       <c r="C67" s="2">
         <v>0.5</v>
       </c>
@@ -15150,7 +15159,7 @@
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="4" t="s">
+      <c r="A68" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B68" s="2">
@@ -15174,7 +15183,7 @@
       <c r="H68" s="3"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="4"/>
+      <c r="A69" s="9"/>
       <c r="B69" s="2">
         <v>2</v>
       </c>
@@ -15196,7 +15205,7 @@
       <c r="H69" s="3"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="4"/>
+      <c r="A70" s="9"/>
       <c r="B70" s="2">
         <v>3</v>
       </c>
@@ -15218,7 +15227,7 @@
       <c r="H70" s="3"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="4"/>
+      <c r="A71" s="9"/>
       <c r="B71" s="2">
         <v>4</v>
       </c>
@@ -15240,7 +15249,7 @@
       <c r="H71" s="3"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="4"/>
+      <c r="A72" s="9"/>
       <c r="B72" s="2">
         <v>5</v>
       </c>
@@ -15262,7 +15271,7 @@
       <c r="H72" s="3"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="4"/>
+      <c r="A73" s="9"/>
       <c r="B73" s="2">
         <v>6</v>
       </c>
@@ -15284,7 +15293,7 @@
       <c r="H73" s="3"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="4"/>
+      <c r="A74" s="9"/>
       <c r="B74" s="2">
         <v>7</v>
       </c>
@@ -15306,7 +15315,7 @@
       <c r="H74" s="3"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="4"/>
+      <c r="A75" s="9"/>
       <c r="B75" s="2">
         <v>8</v>
       </c>
@@ -15328,7 +15337,7 @@
       <c r="H75" s="3"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="4"/>
+      <c r="A76" s="9"/>
       <c r="B76" s="2">
         <v>9</v>
       </c>
@@ -15350,7 +15359,7 @@
       <c r="H76" s="3"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="4"/>
+      <c r="A77" s="9"/>
       <c r="B77" s="2">
         <v>10</v>
       </c>
@@ -15372,22 +15381,22 @@
       <c r="H77" s="3"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" s="5" t="s">
+      <c r="A79" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B79" s="5"/>
-      <c r="C79" s="4" t="s">
+      <c r="B79" s="10"/>
+      <c r="C79" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D79" s="4"/>
-      <c r="E79" s="4"/>
-      <c r="F79" s="4"/>
-      <c r="G79" s="4"/>
-      <c r="H79" s="4"/>
+      <c r="D79" s="9"/>
+      <c r="E79" s="9"/>
+      <c r="F79" s="9"/>
+      <c r="G79" s="9"/>
+      <c r="H79" s="9"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" s="5"/>
-      <c r="B80" s="5"/>
+      <c r="A80" s="10"/>
+      <c r="B80" s="10"/>
       <c r="C80" s="2">
         <v>0.5</v>
       </c>
@@ -15408,7 +15417,7 @@
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" s="4" t="s">
+      <c r="A81" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B81" s="2">
@@ -15432,7 +15441,7 @@
       <c r="H81" s="3"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="4"/>
+      <c r="A82" s="9"/>
       <c r="B82" s="2">
         <v>2</v>
       </c>
@@ -15454,7 +15463,7 @@
       <c r="H82" s="3"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" s="4"/>
+      <c r="A83" s="9"/>
       <c r="B83" s="2">
         <v>3</v>
       </c>
@@ -15476,7 +15485,7 @@
       <c r="H83" s="3"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" s="4"/>
+      <c r="A84" s="9"/>
       <c r="B84" s="2">
         <v>4</v>
       </c>
@@ -15498,7 +15507,7 @@
       <c r="H84" s="3"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" s="4"/>
+      <c r="A85" s="9"/>
       <c r="B85" s="2">
         <v>5</v>
       </c>
@@ -15520,7 +15529,7 @@
       <c r="H85" s="3"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" s="4"/>
+      <c r="A86" s="9"/>
       <c r="B86" s="2">
         <v>6</v>
       </c>
@@ -15542,7 +15551,7 @@
       <c r="H86" s="3"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="4"/>
+      <c r="A87" s="9"/>
       <c r="B87" s="2">
         <v>7</v>
       </c>
@@ -15564,7 +15573,7 @@
       <c r="H87" s="3"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" s="4"/>
+      <c r="A88" s="9"/>
       <c r="B88" s="2">
         <v>8</v>
       </c>
@@ -15586,7 +15595,7 @@
       <c r="H88" s="3"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="4"/>
+      <c r="A89" s="9"/>
       <c r="B89" s="2">
         <v>9</v>
       </c>
@@ -15608,7 +15617,7 @@
       <c r="H89" s="3"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="4"/>
+      <c r="A90" s="9"/>
       <c r="B90" s="2">
         <v>10</v>
       </c>
@@ -15630,22 +15639,22 @@
       <c r="H90" s="3"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" s="5" t="s">
+      <c r="A92" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B92" s="5"/>
-      <c r="C92" s="4" t="s">
+      <c r="B92" s="10"/>
+      <c r="C92" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D92" s="4"/>
-      <c r="E92" s="4"/>
-      <c r="F92" s="4"/>
-      <c r="G92" s="4"/>
-      <c r="H92" s="4"/>
+      <c r="D92" s="9"/>
+      <c r="E92" s="9"/>
+      <c r="F92" s="9"/>
+      <c r="G92" s="9"/>
+      <c r="H92" s="9"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" s="5"/>
-      <c r="B93" s="5"/>
+      <c r="A93" s="10"/>
+      <c r="B93" s="10"/>
       <c r="C93" s="2">
         <v>0.5</v>
       </c>
@@ -15666,7 +15675,7 @@
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" s="4" t="s">
+      <c r="A94" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B94" s="2">
@@ -15690,7 +15699,7 @@
       <c r="H94" s="3"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A95" s="4"/>
+      <c r="A95" s="9"/>
       <c r="B95" s="2">
         <v>2</v>
       </c>
@@ -15712,7 +15721,7 @@
       <c r="H95" s="3"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="4"/>
+      <c r="A96" s="9"/>
       <c r="B96" s="2">
         <v>3</v>
       </c>
@@ -15734,7 +15743,7 @@
       <c r="H96" s="3"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A97" s="4"/>
+      <c r="A97" s="9"/>
       <c r="B97" s="2">
         <v>4</v>
       </c>
@@ -15756,7 +15765,7 @@
       <c r="H97" s="3"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A98" s="4"/>
+      <c r="A98" s="9"/>
       <c r="B98" s="2">
         <v>5</v>
       </c>
@@ -15778,7 +15787,7 @@
       <c r="H98" s="3"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A99" s="4"/>
+      <c r="A99" s="9"/>
       <c r="B99" s="2">
         <v>6</v>
       </c>
@@ -15800,7 +15809,7 @@
       <c r="H99" s="3"/>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A100" s="4"/>
+      <c r="A100" s="9"/>
       <c r="B100" s="2">
         <v>7</v>
       </c>
@@ -15822,7 +15831,7 @@
       <c r="H100" s="3"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A101" s="4"/>
+      <c r="A101" s="9"/>
       <c r="B101" s="2">
         <v>8</v>
       </c>
@@ -15844,7 +15853,7 @@
       <c r="H101" s="3"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A102" s="4"/>
+      <c r="A102" s="9"/>
       <c r="B102" s="2">
         <v>9</v>
       </c>
@@ -15866,7 +15875,7 @@
       <c r="H102" s="3"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A103" s="4"/>
+      <c r="A103" s="9"/>
       <c r="B103" s="2">
         <v>10</v>
       </c>
@@ -15888,22 +15897,22 @@
       <c r="H103" s="3"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A105" s="5" t="s">
+      <c r="A105" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B105" s="5"/>
-      <c r="C105" s="4" t="s">
+      <c r="B105" s="10"/>
+      <c r="C105" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D105" s="4"/>
-      <c r="E105" s="4"/>
-      <c r="F105" s="4"/>
-      <c r="G105" s="4"/>
-      <c r="H105" s="4"/>
+      <c r="D105" s="9"/>
+      <c r="E105" s="9"/>
+      <c r="F105" s="9"/>
+      <c r="G105" s="9"/>
+      <c r="H105" s="9"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A106" s="5"/>
-      <c r="B106" s="5"/>
+      <c r="A106" s="10"/>
+      <c r="B106" s="10"/>
       <c r="C106" s="2">
         <v>0.5</v>
       </c>
@@ -15924,7 +15933,7 @@
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A107" s="4" t="s">
+      <c r="A107" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B107" s="2">
@@ -15948,7 +15957,7 @@
       <c r="H107" s="3"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A108" s="4"/>
+      <c r="A108" s="9"/>
       <c r="B108" s="2">
         <v>2</v>
       </c>
@@ -15970,7 +15979,7 @@
       <c r="H108" s="3"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A109" s="4"/>
+      <c r="A109" s="9"/>
       <c r="B109" s="2">
         <v>3</v>
       </c>
@@ -15992,7 +16001,7 @@
       <c r="H109" s="3"/>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A110" s="4"/>
+      <c r="A110" s="9"/>
       <c r="B110" s="2">
         <v>4</v>
       </c>
@@ -16014,7 +16023,7 @@
       <c r="H110" s="3"/>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A111" s="4"/>
+      <c r="A111" s="9"/>
       <c r="B111" s="2">
         <v>5</v>
       </c>
@@ -16036,7 +16045,7 @@
       <c r="H111" s="3"/>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A112" s="4"/>
+      <c r="A112" s="9"/>
       <c r="B112" s="2">
         <v>6</v>
       </c>
@@ -16058,7 +16067,7 @@
       <c r="H112" s="3"/>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A113" s="4"/>
+      <c r="A113" s="9"/>
       <c r="B113" s="2">
         <v>7</v>
       </c>
@@ -16080,7 +16089,7 @@
       <c r="H113" s="3"/>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A114" s="4"/>
+      <c r="A114" s="9"/>
       <c r="B114" s="2">
         <v>8</v>
       </c>
@@ -16102,7 +16111,7 @@
       <c r="H114" s="3"/>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A115" s="4"/>
+      <c r="A115" s="9"/>
       <c r="B115" s="2">
         <v>9</v>
       </c>
@@ -16124,7 +16133,7 @@
       <c r="H115" s="3"/>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A116" s="4"/>
+      <c r="A116" s="9"/>
       <c r="B116" s="2">
         <v>10</v>
       </c>
@@ -16146,22 +16155,22 @@
       <c r="H116" s="3"/>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A118" s="5" t="s">
+      <c r="A118" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B118" s="5"/>
-      <c r="C118" s="4" t="s">
+      <c r="B118" s="10"/>
+      <c r="C118" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D118" s="4"/>
-      <c r="E118" s="4"/>
-      <c r="F118" s="4"/>
-      <c r="G118" s="4"/>
-      <c r="H118" s="4"/>
+      <c r="D118" s="9"/>
+      <c r="E118" s="9"/>
+      <c r="F118" s="9"/>
+      <c r="G118" s="9"/>
+      <c r="H118" s="9"/>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A119" s="5"/>
-      <c r="B119" s="5"/>
+      <c r="A119" s="10"/>
+      <c r="B119" s="10"/>
       <c r="C119" s="2">
         <v>0.5</v>
       </c>
@@ -16182,7 +16191,7 @@
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A120" s="4" t="s">
+      <c r="A120" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B120" s="2">
@@ -16206,7 +16215,7 @@
       <c r="H120" s="3"/>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A121" s="4"/>
+      <c r="A121" s="9"/>
       <c r="B121" s="2">
         <v>2</v>
       </c>
@@ -16228,7 +16237,7 @@
       <c r="H121" s="3"/>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A122" s="4"/>
+      <c r="A122" s="9"/>
       <c r="B122" s="2">
         <v>3</v>
       </c>
@@ -16250,7 +16259,7 @@
       <c r="H122" s="3"/>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A123" s="4"/>
+      <c r="A123" s="9"/>
       <c r="B123" s="2">
         <v>4</v>
       </c>
@@ -16272,7 +16281,7 @@
       <c r="H123" s="3"/>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A124" s="4"/>
+      <c r="A124" s="9"/>
       <c r="B124" s="2">
         <v>5</v>
       </c>
@@ -16294,7 +16303,7 @@
       <c r="H124" s="3"/>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A125" s="4"/>
+      <c r="A125" s="9"/>
       <c r="B125" s="2">
         <v>6</v>
       </c>
@@ -16316,7 +16325,7 @@
       <c r="H125" s="3"/>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A126" s="4"/>
+      <c r="A126" s="9"/>
       <c r="B126" s="2">
         <v>7</v>
       </c>
@@ -16338,7 +16347,7 @@
       <c r="H126" s="3"/>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A127" s="4"/>
+      <c r="A127" s="9"/>
       <c r="B127" s="2">
         <v>8</v>
       </c>
@@ -16360,7 +16369,7 @@
       <c r="H127" s="3"/>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A128" s="4"/>
+      <c r="A128" s="9"/>
       <c r="B128" s="2">
         <v>9</v>
       </c>
@@ -16382,7 +16391,7 @@
       <c r="H128" s="3"/>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A129" s="4"/>
+      <c r="A129" s="9"/>
       <c r="B129" s="2">
         <v>10</v>
       </c>
@@ -16405,27 +16414,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A3:A12"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="A14:B15"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="C66:H66"/>
-    <mergeCell ref="C53:H53"/>
-    <mergeCell ref="A16:A25"/>
-    <mergeCell ref="A27:B28"/>
-    <mergeCell ref="A29:A38"/>
-    <mergeCell ref="A40:B41"/>
-    <mergeCell ref="C40:H40"/>
-    <mergeCell ref="C27:H27"/>
-    <mergeCell ref="A68:A77"/>
-    <mergeCell ref="A79:B80"/>
-    <mergeCell ref="A81:A90"/>
-    <mergeCell ref="A92:B93"/>
-    <mergeCell ref="A42:A51"/>
-    <mergeCell ref="A53:B54"/>
-    <mergeCell ref="A55:A64"/>
-    <mergeCell ref="A66:B67"/>
     <mergeCell ref="A120:A129"/>
     <mergeCell ref="C118:H118"/>
     <mergeCell ref="C105:H105"/>
@@ -16435,6 +16423,27 @@
     <mergeCell ref="A105:B106"/>
     <mergeCell ref="A107:A116"/>
     <mergeCell ref="A118:B119"/>
+    <mergeCell ref="A68:A77"/>
+    <mergeCell ref="A79:B80"/>
+    <mergeCell ref="A81:A90"/>
+    <mergeCell ref="A92:B93"/>
+    <mergeCell ref="A42:A51"/>
+    <mergeCell ref="A53:B54"/>
+    <mergeCell ref="A55:A64"/>
+    <mergeCell ref="A66:B67"/>
+    <mergeCell ref="C66:H66"/>
+    <mergeCell ref="C53:H53"/>
+    <mergeCell ref="A16:A25"/>
+    <mergeCell ref="A27:B28"/>
+    <mergeCell ref="A29:A38"/>
+    <mergeCell ref="A40:B41"/>
+    <mergeCell ref="C40:H40"/>
+    <mergeCell ref="C27:H27"/>
+    <mergeCell ref="A3:A12"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="A14:B15"/>
+    <mergeCell ref="C14:H14"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:H12 C16:H25 C29:H38 C42:H51 C55:H64 C68:H77 C81:H90 C94:H103 C107:H116 C120:H129">
     <cfRule type="colorScale" priority="1">
@@ -16458,1939 +16467,1991 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E91C0581-E8C2-4506-9305-1F1CBC86D7DE}">
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="AV30" sqref="AV30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="6" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="7.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="4" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="7">
         <v>10.97</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="7">
         <v>5.26</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="7">
         <v>4.51</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="7">
         <v>4.41</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="7">
         <v>4.34</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="7">
         <v>4.6399999999999997</v>
       </c>
-      <c r="H2" s="9">
+      <c r="H2" s="7">
         <v>4.59</v>
       </c>
-      <c r="I2" s="9">
+      <c r="I2" s="7">
         <v>4.82</v>
       </c>
-      <c r="J2" s="9">
+      <c r="J2" s="7">
         <v>4.87</v>
       </c>
-      <c r="K2" s="9">
+      <c r="K2" s="7">
         <v>4.9800000000000004</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="7">
         <v>10.24</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="7">
         <v>4.8</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="7">
         <v>3.99</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="7">
         <v>4.09</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="7">
         <v>3.89</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="7">
         <v>4.08</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="7">
         <v>4.12</v>
       </c>
-      <c r="I3" s="9">
+      <c r="I3" s="7">
         <v>4.37</v>
       </c>
-      <c r="J3" s="9">
+      <c r="J3" s="7">
         <v>4.9000000000000004</v>
       </c>
-      <c r="K3" s="9">
+      <c r="K3" s="7">
         <v>5.42</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="7">
         <v>9.14</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="7">
         <v>4.6500000000000004</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="7">
         <v>3.58</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="7">
         <v>3.64</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="7">
         <v>3.6</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="7">
         <v>4.21</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="7">
         <v>4.3099999999999996</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="7">
         <v>4.72</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J4" s="7">
         <v>4.83</v>
       </c>
-      <c r="K4" s="9">
+      <c r="K4" s="7">
         <v>4.9800000000000004</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="7">
         <v>9.3000000000000007</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="7">
         <v>4.12</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="7">
         <v>4.16</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="7">
         <v>3.58</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="7">
         <v>3.74</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="7">
         <v>4.1900000000000004</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="7">
         <v>3.95</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="7">
         <v>4.34</v>
       </c>
-      <c r="J5" s="9">
+      <c r="J5" s="7">
         <v>4.84</v>
       </c>
-      <c r="K5" s="9">
+      <c r="K5" s="7">
         <v>5.34</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="7">
         <v>9.3000000000000007</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="7">
         <v>3.81</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="7">
         <v>3.68</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="7">
         <v>3.28</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="7">
         <v>3.43</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="7">
         <v>3.55</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="7">
         <v>4.16</v>
       </c>
-      <c r="I6" s="9">
+      <c r="I6" s="7">
         <v>4.0999999999999996</v>
       </c>
-      <c r="J6" s="9">
+      <c r="J6" s="7">
         <v>4.55</v>
       </c>
-      <c r="K6" s="9">
+      <c r="K6" s="7">
         <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="7">
         <v>8.82</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="7">
         <v>4.28</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="7">
         <v>3.18</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="7">
         <v>3.19</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="7">
         <v>2.84</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="7">
         <v>3.42</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="7">
         <v>3.77</v>
       </c>
-      <c r="I7" s="9">
+      <c r="I7" s="7">
         <v>3.91</v>
       </c>
-      <c r="J7" s="9">
+      <c r="J7" s="7">
         <v>4.21</v>
       </c>
-      <c r="K7" s="9">
+      <c r="K7" s="7">
         <v>4.74</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="7">
         <v>8.92</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="7">
         <v>4.21</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="7">
         <v>3.54</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="7">
         <v>3.12</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="7">
         <v>3.31</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="7">
         <v>3.68</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="7">
         <v>4.1500000000000004</v>
       </c>
-      <c r="I8" s="9">
+      <c r="I8" s="7">
         <v>4.24</v>
       </c>
-      <c r="J8" s="9">
+      <c r="J8" s="7">
         <v>3.97</v>
       </c>
-      <c r="K8" s="9">
+      <c r="K8" s="7">
         <v>4.54</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="7">
         <v>8.1300000000000008</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="7">
         <v>3.8</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="7">
         <v>2.87</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="7">
         <v>2.89</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="7">
         <v>2.89</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="7">
         <v>3.28</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="7">
         <v>3.59</v>
       </c>
-      <c r="I9" s="9">
+      <c r="I9" s="7">
         <v>4.12</v>
       </c>
-      <c r="J9" s="9">
+      <c r="J9" s="7">
         <v>4.7699999999999996</v>
       </c>
-      <c r="K9" s="9">
+      <c r="K9" s="7">
         <v>4.6100000000000003</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="7">
         <v>8.4</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="7">
         <v>3.64</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="7">
         <v>2.98</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="7">
         <v>2.98</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="7">
         <v>3.35</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="7">
         <v>3.51</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="7">
         <v>4.0599999999999996</v>
       </c>
-      <c r="I10" s="9">
+      <c r="I10" s="7">
         <v>4.24</v>
       </c>
-      <c r="J10" s="9">
+      <c r="J10" s="7">
         <v>4.59</v>
       </c>
-      <c r="K10" s="9">
+      <c r="K10" s="7">
         <v>4.8099999999999996</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="7">
         <v>8.4700000000000006</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="7">
         <v>3.72</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="7">
         <v>2.93</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="7">
         <v>3.41</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="7">
         <v>3.45</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="7">
         <v>3.31</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H11" s="7">
         <v>3.7</v>
       </c>
-      <c r="I11" s="9">
+      <c r="I11" s="7">
         <v>4.34</v>
       </c>
-      <c r="J11" s="9">
+      <c r="J11" s="7">
         <v>4.28</v>
       </c>
-      <c r="K11" s="9">
+      <c r="K11" s="7">
         <v>4.3099999999999996</v>
       </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="H13" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="I13" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="J13" s="8" t="s">
+      <c r="J13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K13" s="8" t="s">
+      <c r="K13" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="7">
         <v>10.83</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="7">
         <v>5.07</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="7">
         <v>4.16</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="7">
         <v>4.05</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="7">
         <v>3.96</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="7">
         <v>4.24</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H14" s="7">
         <v>4.21</v>
       </c>
-      <c r="I14" s="9">
+      <c r="I14" s="7">
         <v>4.43</v>
       </c>
-      <c r="J14" s="9">
+      <c r="J14" s="7">
         <v>4.45</v>
       </c>
-      <c r="K14" s="9">
+      <c r="K14" s="7">
         <v>4.68</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="7">
         <v>10.08</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="7">
         <v>4.82</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="7">
         <v>3.87</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="7">
         <v>3.69</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="7">
         <v>3.64</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="7">
         <v>3.87</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="7">
         <v>4.07</v>
       </c>
-      <c r="I15" s="9">
+      <c r="I15" s="7">
         <v>4.21</v>
       </c>
-      <c r="J15" s="9">
+      <c r="J15" s="7">
         <v>4.82</v>
       </c>
-      <c r="K15" s="9">
+      <c r="K15" s="7">
         <v>5.08</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="7">
         <v>8.6300000000000008</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="7">
         <v>4.38</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="7">
         <v>3.52</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="7">
         <v>3.26</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="7">
         <v>3.37</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="7">
         <v>3.7</v>
       </c>
-      <c r="H16" s="9">
+      <c r="H16" s="7">
         <v>3.96</v>
       </c>
-      <c r="I16" s="9">
+      <c r="I16" s="7">
         <v>4.0999999999999996</v>
       </c>
-      <c r="J16" s="9">
+      <c r="J16" s="7">
         <v>4.18</v>
       </c>
-      <c r="K16" s="9">
+      <c r="K16" s="7">
         <v>4.78</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="7">
         <v>8.81</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="7">
         <v>3.91</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="7">
         <v>3.52</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="7">
         <v>3.34</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="7">
         <v>3.24</v>
       </c>
-      <c r="G17" s="9">
+      <c r="G17" s="7">
         <v>3.49</v>
       </c>
-      <c r="H17" s="9">
+      <c r="H17" s="7">
         <v>3.66</v>
       </c>
-      <c r="I17" s="9">
+      <c r="I17" s="7">
         <v>4.3</v>
       </c>
-      <c r="J17" s="9">
+      <c r="J17" s="7">
         <v>4.54</v>
       </c>
-      <c r="K17" s="9">
+      <c r="K17" s="7">
         <v>5.17</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="7">
         <v>8.94</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="7">
         <v>3.38</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="7">
         <v>3.33</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="7">
         <v>3</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="7">
         <v>3.11</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="7">
         <v>3.14</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H18" s="7">
         <v>3.73</v>
       </c>
-      <c r="I18" s="9">
+      <c r="I18" s="7">
         <v>3.97</v>
       </c>
-      <c r="J18" s="9">
+      <c r="J18" s="7">
         <v>4.2</v>
       </c>
-      <c r="K18" s="9">
+      <c r="K18" s="7">
         <v>4.63</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="7">
         <v>8.1300000000000008</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="7">
         <v>3.82</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="7">
         <v>2.97</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19" s="7">
         <v>2.73</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="7">
         <v>2.77</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G19" s="7">
         <v>3.34</v>
       </c>
-      <c r="H19" s="9">
+      <c r="H19" s="7">
         <v>3.19</v>
       </c>
-      <c r="I19" s="9">
+      <c r="I19" s="7">
         <v>3.56</v>
       </c>
-      <c r="J19" s="9">
+      <c r="J19" s="7">
         <v>3.65</v>
       </c>
-      <c r="K19" s="9">
+      <c r="K19" s="7">
         <v>4.22</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20" s="7">
         <v>8.33</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="7">
         <v>3.69</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="7">
         <v>2.81</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="7">
         <v>2.93</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="7">
         <v>2.86</v>
       </c>
-      <c r="G20" s="9">
+      <c r="G20" s="7">
         <v>3.08</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H20" s="7">
         <v>3.55</v>
       </c>
-      <c r="I20" s="9">
+      <c r="I20" s="7">
         <v>3.58</v>
       </c>
-      <c r="J20" s="9">
+      <c r="J20" s="7">
         <v>3.73</v>
       </c>
-      <c r="K20" s="9">
+      <c r="K20" s="7">
         <v>3.97</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B21" s="7">
         <v>7.63</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="7">
         <v>3.59</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D21" s="7">
         <v>2.64</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="7">
         <v>2.59</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21" s="7">
         <v>2.76</v>
       </c>
-      <c r="G21" s="9">
+      <c r="G21" s="7">
         <v>3</v>
       </c>
-      <c r="H21" s="9">
+      <c r="H21" s="7">
         <v>3.23</v>
       </c>
-      <c r="I21" s="9">
+      <c r="I21" s="7">
         <v>3.75</v>
       </c>
-      <c r="J21" s="9">
+      <c r="J21" s="7">
         <v>4.42</v>
       </c>
-      <c r="K21" s="9">
+      <c r="K21" s="7">
         <v>4.41</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="9">
+      <c r="B22" s="7">
         <v>7.68</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C22" s="7">
         <v>3.39</v>
       </c>
-      <c r="D22" s="9">
+      <c r="D22" s="7">
         <v>2.82</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E22" s="7">
         <v>2.5299999999999998</v>
       </c>
-      <c r="F22" s="9">
+      <c r="F22" s="7">
         <v>2.84</v>
       </c>
-      <c r="G22" s="9">
+      <c r="G22" s="7">
         <v>3.36</v>
       </c>
-      <c r="H22" s="9">
+      <c r="H22" s="7">
         <v>3.08</v>
       </c>
-      <c r="I22" s="9">
+      <c r="I22" s="7">
         <v>3.29</v>
       </c>
-      <c r="J22" s="9">
+      <c r="J22" s="7">
         <v>3.99</v>
       </c>
-      <c r="K22" s="9">
+      <c r="K22" s="7">
         <v>4.22</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="9">
+      <c r="B23" s="7">
         <v>7.8</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C23" s="7">
         <v>3.3</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23" s="7">
         <v>2.81</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E23" s="7">
         <v>2.59</v>
       </c>
-      <c r="F23" s="9">
+      <c r="F23" s="7">
         <v>2.93</v>
       </c>
-      <c r="G23" s="9">
+      <c r="G23" s="7">
         <v>3</v>
       </c>
-      <c r="H23" s="9">
+      <c r="H23" s="7">
         <v>3.38</v>
       </c>
-      <c r="I23" s="9">
+      <c r="I23" s="7">
         <v>3.47</v>
       </c>
-      <c r="J23" s="9">
+      <c r="J23" s="7">
         <v>3.9</v>
       </c>
-      <c r="K23" s="9">
+      <c r="K23" s="7">
         <v>3.95</v>
       </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="F25" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G25" s="8" t="s">
+      <c r="G25" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H25" s="8" t="s">
+      <c r="H25" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I25" s="8" t="s">
+      <c r="I25" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="J25" s="8" t="s">
+      <c r="J25" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K25" s="8" t="s">
+      <c r="K25" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="9">
+      <c r="B26" s="7">
         <v>10.82</v>
       </c>
-      <c r="C26" s="9">
+      <c r="C26" s="7">
         <v>4.97</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D26" s="7">
         <v>3.99</v>
       </c>
-      <c r="E26" s="9">
+      <c r="E26" s="7">
         <v>3.85</v>
       </c>
-      <c r="F26" s="9">
+      <c r="F26" s="7">
         <v>3.7</v>
       </c>
-      <c r="G26" s="9">
+      <c r="G26" s="7">
         <v>3.95</v>
       </c>
-      <c r="H26" s="9">
+      <c r="H26" s="7">
         <v>3.92</v>
       </c>
-      <c r="I26" s="9">
+      <c r="I26" s="7">
         <v>4.0999999999999996</v>
       </c>
-      <c r="J26" s="9">
+      <c r="J26" s="7">
         <v>4.12</v>
       </c>
-      <c r="K26" s="9">
+      <c r="K26" s="7">
         <v>4.42</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="9">
+      <c r="B27" s="7">
         <v>9.6999999999999993</v>
       </c>
-      <c r="C27" s="9">
+      <c r="C27" s="7">
         <v>4.63</v>
       </c>
-      <c r="D27" s="9">
+      <c r="D27" s="7">
         <v>3.72</v>
       </c>
-      <c r="E27" s="9">
+      <c r="E27" s="7">
         <v>3.34</v>
       </c>
-      <c r="F27" s="9">
+      <c r="F27" s="7">
         <v>3.46</v>
       </c>
-      <c r="G27" s="9">
+      <c r="G27" s="7">
         <v>3.64</v>
       </c>
-      <c r="H27" s="9">
+      <c r="H27" s="7">
         <v>3.99</v>
       </c>
-      <c r="I27" s="9">
+      <c r="I27" s="7">
         <v>4.0999999999999996</v>
       </c>
-      <c r="J27" s="9">
+      <c r="J27" s="7">
         <v>4.97</v>
       </c>
-      <c r="K27" s="9">
+      <c r="K27" s="7">
         <v>5.18</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B28" s="9">
+      <c r="B28" s="7">
         <v>8.6199999999999992</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C28" s="7">
         <v>4.28</v>
       </c>
-      <c r="D28" s="9">
+      <c r="D28" s="7">
         <v>3.3</v>
       </c>
-      <c r="E28" s="9">
+      <c r="E28" s="7">
         <v>2.97</v>
       </c>
-      <c r="F28" s="9">
+      <c r="F28" s="7">
         <v>3.23</v>
       </c>
-      <c r="G28" s="9">
+      <c r="G28" s="7">
         <v>3.38</v>
       </c>
-      <c r="H28" s="9">
+      <c r="H28" s="7">
         <v>3.65</v>
       </c>
-      <c r="I28" s="9">
+      <c r="I28" s="7">
         <v>3.74</v>
       </c>
-      <c r="J28" s="9">
+      <c r="J28" s="7">
         <v>4.0599999999999996</v>
       </c>
-      <c r="K28" s="9">
+      <c r="K28" s="7">
         <v>4.84</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="9">
+      <c r="B29" s="7">
         <v>8.68</v>
       </c>
-      <c r="C29" s="9">
+      <c r="C29" s="7">
         <v>3.67</v>
       </c>
-      <c r="D29" s="9">
+      <c r="D29" s="7">
         <v>3.27</v>
       </c>
-      <c r="E29" s="9">
+      <c r="E29" s="7">
         <v>3</v>
       </c>
-      <c r="F29" s="9">
+      <c r="F29" s="7">
         <v>3.06</v>
       </c>
-      <c r="G29" s="9">
+      <c r="G29" s="7">
         <v>3.39</v>
       </c>
-      <c r="H29" s="9">
+      <c r="H29" s="7">
         <v>3.51</v>
       </c>
-      <c r="I29" s="9">
+      <c r="I29" s="7">
         <v>3.85</v>
       </c>
-      <c r="J29" s="9">
+      <c r="J29" s="7">
         <v>4.49</v>
       </c>
-      <c r="K29" s="9">
+      <c r="K29" s="7">
         <v>5.54</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="9">
+      <c r="B30" s="7">
         <v>8.0399999999999991</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C30" s="7">
         <v>3.44</v>
       </c>
-      <c r="D30" s="9">
+      <c r="D30" s="7">
         <v>2.95</v>
       </c>
-      <c r="E30" s="9">
+      <c r="E30" s="7">
         <v>2.91</v>
       </c>
-      <c r="F30" s="9">
+      <c r="F30" s="7">
         <v>2.85</v>
       </c>
-      <c r="G30" s="9">
+      <c r="G30" s="7">
         <v>3.06</v>
       </c>
-      <c r="H30" s="9">
+      <c r="H30" s="7">
         <v>3.37</v>
       </c>
-      <c r="I30" s="9">
+      <c r="I30" s="7">
         <v>3.71</v>
       </c>
-      <c r="J30" s="9">
+      <c r="J30" s="7">
         <v>4.21</v>
       </c>
-      <c r="K30" s="9">
+      <c r="K30" s="7">
         <v>4.83</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B31" s="9">
+      <c r="B31" s="7">
         <v>7.68</v>
       </c>
-      <c r="C31" s="9">
+      <c r="C31" s="7">
         <v>3.6</v>
       </c>
-      <c r="D31" s="9">
+      <c r="D31" s="7">
         <v>2.66</v>
       </c>
-      <c r="E31" s="9">
+      <c r="E31" s="7">
         <v>2.5</v>
       </c>
-      <c r="F31" s="9">
+      <c r="F31" s="7">
         <v>2.37</v>
       </c>
-      <c r="G31" s="9">
+      <c r="G31" s="7">
         <v>3.04</v>
       </c>
-      <c r="H31" s="9">
+      <c r="H31" s="7">
         <v>3.06</v>
       </c>
-      <c r="I31" s="9">
+      <c r="I31" s="7">
         <v>3.69</v>
       </c>
-      <c r="J31" s="9">
+      <c r="J31" s="7">
         <v>3.8</v>
       </c>
-      <c r="K31" s="9">
+      <c r="K31" s="7">
         <v>4.3</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
+      <c r="A32" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B32" s="9">
+      <c r="B32" s="7">
         <v>7.87</v>
       </c>
-      <c r="C32" s="9">
+      <c r="C32" s="7">
         <v>3.29</v>
       </c>
-      <c r="D32" s="9">
+      <c r="D32" s="7">
         <v>2.75</v>
       </c>
-      <c r="E32" s="9">
+      <c r="E32" s="7">
         <v>2.64</v>
       </c>
-      <c r="F32" s="9">
+      <c r="F32" s="7">
         <v>2.78</v>
       </c>
-      <c r="G32" s="9">
+      <c r="G32" s="7">
         <v>2.75</v>
       </c>
-      <c r="H32" s="9">
+      <c r="H32" s="7">
         <v>3.05</v>
       </c>
-      <c r="I32" s="9">
+      <c r="I32" s="7">
         <v>3.75</v>
       </c>
-      <c r="J32" s="9">
+      <c r="J32" s="7">
         <v>3.77</v>
       </c>
-      <c r="K32" s="9">
+      <c r="K32" s="7">
         <v>4.07</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
+      <c r="A33" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="9">
+      <c r="B33" s="7">
         <v>7.29</v>
       </c>
-      <c r="C33" s="9">
+      <c r="C33" s="7">
         <v>3.2</v>
       </c>
-      <c r="D33" s="9">
+      <c r="D33" s="7">
         <v>2.36</v>
       </c>
-      <c r="E33" s="9">
+      <c r="E33" s="7">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F33" s="9">
+      <c r="F33" s="7">
         <v>2.54</v>
       </c>
-      <c r="G33" s="9">
+      <c r="G33" s="7">
         <v>2.7</v>
       </c>
-      <c r="H33" s="9">
+      <c r="H33" s="7">
         <v>2.73</v>
       </c>
-      <c r="I33" s="9">
+      <c r="I33" s="7">
         <v>3.49</v>
       </c>
-      <c r="J33" s="9">
+      <c r="J33" s="7">
         <v>4.12</v>
       </c>
-      <c r="K33" s="9">
+      <c r="K33" s="7">
         <v>4.2</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B34" s="9">
+      <c r="B34" s="7">
         <v>7.07</v>
       </c>
-      <c r="C34" s="9">
+      <c r="C34" s="7">
         <v>3.3</v>
       </c>
-      <c r="D34" s="9">
+      <c r="D34" s="7">
         <v>2.64</v>
       </c>
-      <c r="E34" s="10">
+      <c r="E34" s="8">
         <v>2.2000000000000002</v>
       </c>
-      <c r="F34" s="9">
+      <c r="F34" s="7">
         <v>2.56</v>
       </c>
-      <c r="G34" s="9">
+      <c r="G34" s="7">
         <v>3.13</v>
       </c>
-      <c r="H34" s="9">
+      <c r="H34" s="7">
         <v>3</v>
       </c>
-      <c r="I34" s="9">
+      <c r="I34" s="7">
         <v>3.01</v>
       </c>
-      <c r="J34" s="9">
+      <c r="J34" s="7">
         <v>3.51</v>
       </c>
-      <c r="K34" s="9">
+      <c r="K34" s="7">
         <v>3.76</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
+      <c r="A35" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B35" s="9">
+      <c r="B35" s="7">
         <v>7.16</v>
       </c>
-      <c r="C35" s="9">
+      <c r="C35" s="7">
         <v>2.96</v>
       </c>
-      <c r="D35" s="9">
+      <c r="D35" s="7">
         <v>2.75</v>
       </c>
-      <c r="E35" s="9">
+      <c r="E35" s="7">
         <v>2.4500000000000002</v>
       </c>
-      <c r="F35" s="9">
+      <c r="F35" s="7">
         <v>2.65</v>
       </c>
-      <c r="G35" s="9">
+      <c r="G35" s="7">
         <v>2.85</v>
       </c>
-      <c r="H35" s="9">
+      <c r="H35" s="7">
         <v>3.29</v>
       </c>
-      <c r="I35" s="9">
+      <c r="I35" s="7">
         <v>3.33</v>
       </c>
-      <c r="J35" s="9">
+      <c r="J35" s="7">
         <v>3.66</v>
       </c>
-      <c r="K35" s="9">
+      <c r="K35" s="7">
         <v>3.73</v>
       </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="11"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="11"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="D37" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E37" s="8" t="s">
+      <c r="E37" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F37" s="8" t="s">
+      <c r="F37" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G37" s="8" t="s">
+      <c r="G37" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H37" s="8" t="s">
+      <c r="H37" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I37" s="8" t="s">
+      <c r="I37" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="J37" s="8" t="s">
+      <c r="J37" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K37" s="8" t="s">
+      <c r="K37" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
+      <c r="A38" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B38" s="9">
+      <c r="B38" s="7">
         <v>10.82</v>
       </c>
-      <c r="C38" s="9">
+      <c r="C38" s="7">
         <v>4.9800000000000004</v>
       </c>
-      <c r="D38" s="9">
+      <c r="D38" s="7">
         <v>3.99</v>
       </c>
-      <c r="E38" s="9">
+      <c r="E38" s="7">
         <v>3.78</v>
       </c>
-      <c r="F38" s="9">
+      <c r="F38" s="7">
         <v>3.7</v>
       </c>
-      <c r="G38" s="9">
+      <c r="G38" s="7">
         <v>3.92</v>
       </c>
-      <c r="H38" s="9">
+      <c r="H38" s="7">
         <v>3.88</v>
       </c>
-      <c r="I38" s="9">
+      <c r="I38" s="7">
         <v>4.03</v>
       </c>
-      <c r="J38" s="9">
+      <c r="J38" s="7">
         <v>4.07</v>
       </c>
-      <c r="K38" s="9">
+      <c r="K38" s="7">
         <v>4.34</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
+      <c r="A39" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B39" s="9">
+      <c r="B39" s="7">
         <v>9.61</v>
       </c>
-      <c r="C39" s="9">
+      <c r="C39" s="7">
         <v>4.5999999999999996</v>
       </c>
-      <c r="D39" s="9">
+      <c r="D39" s="7">
         <v>3.76</v>
       </c>
-      <c r="E39" s="9">
+      <c r="E39" s="7">
         <v>3.22</v>
       </c>
-      <c r="F39" s="9">
+      <c r="F39" s="7">
         <v>3.41</v>
       </c>
-      <c r="G39" s="9">
+      <c r="G39" s="7">
         <v>3.67</v>
       </c>
-      <c r="H39" s="9">
+      <c r="H39" s="7">
         <v>3.96</v>
       </c>
-      <c r="I39" s="9">
+      <c r="I39" s="7">
         <v>4.08</v>
       </c>
-      <c r="J39" s="9">
+      <c r="J39" s="7">
         <v>5.04</v>
       </c>
-      <c r="K39" s="9">
+      <c r="K39" s="7">
         <v>5.34</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
+      <c r="A40" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B40" s="9">
+      <c r="B40" s="7">
         <v>8.5399999999999991</v>
       </c>
-      <c r="C40" s="9">
+      <c r="C40" s="7">
         <v>4.2</v>
       </c>
-      <c r="D40" s="9">
+      <c r="D40" s="7">
         <v>3.15</v>
       </c>
-      <c r="E40" s="9">
+      <c r="E40" s="7">
         <v>2.97</v>
       </c>
-      <c r="F40" s="9">
+      <c r="F40" s="7">
         <v>3.26</v>
       </c>
-      <c r="G40" s="9">
+      <c r="G40" s="7">
         <v>3.37</v>
       </c>
-      <c r="H40" s="9">
+      <c r="H40" s="7">
         <v>3.6</v>
       </c>
-      <c r="I40" s="9">
+      <c r="I40" s="7">
         <v>3.73</v>
       </c>
-      <c r="J40" s="9">
+      <c r="J40" s="7">
         <v>4.04</v>
       </c>
-      <c r="K40" s="9">
+      <c r="K40" s="7">
         <v>4.82</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
+      <c r="A41" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B41" s="9">
+      <c r="B41" s="7">
         <v>8.44</v>
       </c>
-      <c r="C41" s="9">
+      <c r="C41" s="7">
         <v>3.61</v>
       </c>
-      <c r="D41" s="9">
+      <c r="D41" s="7">
         <v>3.19</v>
       </c>
-      <c r="E41" s="9">
+      <c r="E41" s="7">
         <v>2.9</v>
       </c>
-      <c r="F41" s="9">
+      <c r="F41" s="7">
         <v>2.88</v>
       </c>
-      <c r="G41" s="9">
+      <c r="G41" s="7">
         <v>3.25</v>
       </c>
-      <c r="H41" s="9">
+      <c r="H41" s="7">
         <v>3.4</v>
       </c>
-      <c r="I41" s="9">
+      <c r="I41" s="7">
         <v>3.77</v>
       </c>
-      <c r="J41" s="9">
+      <c r="J41" s="7">
         <v>4.67</v>
       </c>
-      <c r="K41" s="9">
+      <c r="K41" s="7">
         <v>5.62</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="8" t="s">
+      <c r="A42" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B42" s="9">
+      <c r="B42" s="7">
         <v>7.86</v>
       </c>
-      <c r="C42" s="9">
+      <c r="C42" s="7">
         <v>3.46</v>
       </c>
-      <c r="D42" s="9">
+      <c r="D42" s="7">
         <v>2.82</v>
       </c>
-      <c r="E42" s="9">
+      <c r="E42" s="7">
         <v>2.88</v>
       </c>
-      <c r="F42" s="9">
+      <c r="F42" s="7">
         <v>2.84</v>
       </c>
-      <c r="G42" s="9">
+      <c r="G42" s="7">
         <v>3.13</v>
       </c>
-      <c r="H42" s="9">
+      <c r="H42" s="7">
         <v>3.36</v>
       </c>
-      <c r="I42" s="9">
+      <c r="I42" s="7">
         <v>3.7</v>
       </c>
-      <c r="J42" s="9">
+      <c r="J42" s="7">
         <v>4.17</v>
       </c>
-      <c r="K42" s="9">
+      <c r="K42" s="7">
         <v>4.93</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="8" t="s">
+      <c r="A43" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B43" s="9">
+      <c r="B43" s="7">
         <v>7.61</v>
       </c>
-      <c r="C43" s="9">
+      <c r="C43" s="7">
         <v>3.29</v>
       </c>
-      <c r="D43" s="9">
+      <c r="D43" s="7">
         <v>2.5299999999999998</v>
       </c>
-      <c r="E43" s="9">
+      <c r="E43" s="7">
         <v>2.46</v>
       </c>
-      <c r="F43" s="9">
+      <c r="F43" s="7">
         <v>2.29</v>
       </c>
-      <c r="G43" s="9">
+      <c r="G43" s="7">
         <v>2.93</v>
       </c>
-      <c r="H43" s="9">
+      <c r="H43" s="7">
         <v>3.02</v>
       </c>
-      <c r="I43" s="9">
+      <c r="I43" s="7">
         <v>3.79</v>
       </c>
-      <c r="J43" s="9">
+      <c r="J43" s="7">
         <v>3.75</v>
       </c>
-      <c r="K43" s="9">
+      <c r="K43" s="7">
         <v>4.24</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="8" t="s">
+      <c r="A44" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B44" s="9">
+      <c r="B44" s="7">
         <v>7.73</v>
       </c>
-      <c r="C44" s="9">
+      <c r="C44" s="7">
         <v>3.19</v>
       </c>
-      <c r="D44" s="9">
+      <c r="D44" s="7">
         <v>2.65</v>
       </c>
-      <c r="E44" s="9">
+      <c r="E44" s="7">
         <v>2.4500000000000002</v>
       </c>
-      <c r="F44" s="9">
+      <c r="F44" s="7">
         <v>2.74</v>
       </c>
-      <c r="G44" s="9">
+      <c r="G44" s="7">
         <v>2.81</v>
       </c>
-      <c r="H44" s="9">
+      <c r="H44" s="7">
         <v>3.03</v>
       </c>
-      <c r="I44" s="9">
+      <c r="I44" s="7">
         <v>3.66</v>
       </c>
-      <c r="J44" s="9">
+      <c r="J44" s="7">
         <v>3.91</v>
       </c>
-      <c r="K44" s="9">
+      <c r="K44" s="7">
         <v>4.1399999999999997</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="8" t="s">
+      <c r="A45" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B45" s="9">
+      <c r="B45" s="7">
         <v>7.45</v>
       </c>
-      <c r="C45" s="9">
+      <c r="C45" s="7">
         <v>3.07</v>
       </c>
-      <c r="D45" s="9">
+      <c r="D45" s="7">
         <v>2.36</v>
       </c>
-      <c r="E45" s="9">
+      <c r="E45" s="7">
         <v>2.4300000000000002</v>
       </c>
-      <c r="F45" s="9">
+      <c r="F45" s="7">
         <v>2.52</v>
       </c>
-      <c r="G45" s="9">
+      <c r="G45" s="7">
         <v>2.74</v>
       </c>
-      <c r="H45" s="9">
+      <c r="H45" s="7">
         <v>2.66</v>
       </c>
-      <c r="I45" s="9">
+      <c r="I45" s="7">
         <v>3.53</v>
       </c>
-      <c r="J45" s="9">
+      <c r="J45" s="7">
         <v>3.99</v>
       </c>
-      <c r="K45" s="9">
+      <c r="K45" s="7">
         <v>4.28</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="8" t="s">
+      <c r="A46" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B46" s="9">
+      <c r="B46" s="7">
         <v>6.92</v>
       </c>
-      <c r="C46" s="9">
+      <c r="C46" s="7">
         <v>3.31</v>
       </c>
-      <c r="D46" s="9">
+      <c r="D46" s="7">
         <v>2.58</v>
       </c>
-      <c r="E46" s="9">
+      <c r="E46" s="7">
         <v>2.29</v>
       </c>
-      <c r="F46" s="9">
+      <c r="F46" s="7">
         <v>2.4</v>
       </c>
-      <c r="G46" s="9">
+      <c r="G46" s="7">
         <v>2.98</v>
       </c>
-      <c r="H46" s="9">
+      <c r="H46" s="7">
         <v>2.88</v>
       </c>
-      <c r="I46" s="9">
+      <c r="I46" s="7">
         <v>2.98</v>
       </c>
-      <c r="J46" s="9">
+      <c r="J46" s="7">
         <v>3.39</v>
       </c>
-      <c r="K46" s="9">
+      <c r="K46" s="7">
         <v>3.73</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="8" t="s">
+      <c r="A47" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B47" s="9">
+      <c r="B47" s="7">
         <v>6.89</v>
       </c>
-      <c r="C47" s="9">
+      <c r="C47" s="7">
         <v>3</v>
       </c>
-      <c r="D47" s="9">
+      <c r="D47" s="7">
         <v>2.6</v>
       </c>
-      <c r="E47" s="9">
+      <c r="E47" s="7">
         <v>2.4</v>
       </c>
-      <c r="F47" s="9">
+      <c r="F47" s="7">
         <v>2.65</v>
       </c>
-      <c r="G47" s="9">
+      <c r="G47" s="7">
         <v>2.94</v>
       </c>
-      <c r="H47" s="9">
+      <c r="H47" s="7">
         <v>3.29</v>
       </c>
-      <c r="I47" s="9">
+      <c r="I47" s="7">
         <v>3.15</v>
       </c>
-      <c r="J47" s="9">
+      <c r="J47" s="7">
         <v>3.54</v>
       </c>
-      <c r="K47" s="9">
+      <c r="K47" s="7">
         <v>3.8</v>
       </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="11"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="11"/>
+      <c r="J48" s="11"/>
+      <c r="K48" s="11"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="B49" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C49" s="8" t="s">
+      <c r="C49" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D49" s="8" t="s">
+      <c r="D49" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E49" s="8" t="s">
+      <c r="E49" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F49" s="8" t="s">
+      <c r="F49" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G49" s="8" t="s">
+      <c r="G49" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H49" s="8" t="s">
+      <c r="H49" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I49" s="8" t="s">
+      <c r="I49" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="J49" s="8" t="s">
+      <c r="J49" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K49" s="8" t="s">
+      <c r="K49" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="8" t="s">
+      <c r="A50" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B50" s="9">
+      <c r="B50" s="7">
         <v>10.81</v>
       </c>
-      <c r="C50" s="9">
+      <c r="C50" s="7">
         <v>4.9800000000000004</v>
       </c>
-      <c r="D50" s="9">
+      <c r="D50" s="7">
         <v>3.92</v>
       </c>
-      <c r="E50" s="9">
+      <c r="E50" s="7">
         <v>3.77</v>
       </c>
-      <c r="F50" s="9">
+      <c r="F50" s="7">
         <v>3.63</v>
       </c>
-      <c r="G50" s="9">
+      <c r="G50" s="7">
         <v>3.9</v>
       </c>
-      <c r="H50" s="9">
+      <c r="H50" s="7">
         <v>3.86</v>
       </c>
-      <c r="I50" s="9">
+      <c r="I50" s="7">
         <v>3.99</v>
       </c>
-      <c r="J50" s="9">
+      <c r="J50" s="7">
         <v>4.09</v>
       </c>
-      <c r="K50" s="9">
+      <c r="K50" s="7">
         <v>4.29</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="8" t="s">
+      <c r="A51" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B51" s="9">
+      <c r="B51" s="7">
         <v>9.69</v>
       </c>
-      <c r="C51" s="9">
+      <c r="C51" s="7">
         <v>4.57</v>
       </c>
-      <c r="D51" s="9">
+      <c r="D51" s="7">
         <v>3.75</v>
       </c>
-      <c r="E51" s="9">
+      <c r="E51" s="7">
         <v>3.2</v>
       </c>
-      <c r="F51" s="9">
+      <c r="F51" s="7">
         <v>3.34</v>
       </c>
-      <c r="G51" s="9">
+      <c r="G51" s="7">
         <v>3.68</v>
       </c>
-      <c r="H51" s="9">
+      <c r="H51" s="7">
         <v>3.96</v>
       </c>
-      <c r="I51" s="9">
+      <c r="I51" s="7">
         <v>4.1100000000000003</v>
       </c>
-      <c r="J51" s="9">
+      <c r="J51" s="7">
         <v>5.03</v>
       </c>
-      <c r="K51" s="9">
+      <c r="K51" s="7">
         <v>5.39</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="8" t="s">
+      <c r="A52" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B52" s="9">
+      <c r="B52" s="7">
         <v>8.6199999999999992</v>
       </c>
-      <c r="C52" s="9">
+      <c r="C52" s="7">
         <v>4.1900000000000004</v>
       </c>
-      <c r="D52" s="9">
+      <c r="D52" s="7">
         <v>3.09</v>
       </c>
-      <c r="E52" s="9">
+      <c r="E52" s="7">
         <v>3.06</v>
       </c>
-      <c r="F52" s="9">
+      <c r="F52" s="7">
         <v>3.21</v>
       </c>
-      <c r="G52" s="9">
+      <c r="G52" s="7">
         <v>3.29</v>
       </c>
-      <c r="H52" s="9">
+      <c r="H52" s="7">
         <v>3.54</v>
       </c>
-      <c r="I52" s="9">
+      <c r="I52" s="7">
         <v>3.76</v>
       </c>
-      <c r="J52" s="9">
+      <c r="J52" s="7">
         <v>4.1399999999999997</v>
       </c>
-      <c r="K52" s="9">
+      <c r="K52" s="7">
         <v>4.8600000000000003</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="8" t="s">
+      <c r="A53" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B53" s="9">
+      <c r="B53" s="7">
         <v>8.33</v>
       </c>
-      <c r="C53" s="9">
+      <c r="C53" s="7">
         <v>3.55</v>
       </c>
-      <c r="D53" s="9">
+      <c r="D53" s="7">
         <v>3.14</v>
       </c>
-      <c r="E53" s="9">
+      <c r="E53" s="7">
         <v>2.83</v>
       </c>
-      <c r="F53" s="9">
+      <c r="F53" s="7">
         <v>2.74</v>
       </c>
-      <c r="G53" s="9">
+      <c r="G53" s="7">
         <v>3.24</v>
       </c>
-      <c r="H53" s="9">
+      <c r="H53" s="7">
         <v>3.34</v>
       </c>
-      <c r="I53" s="9">
+      <c r="I53" s="7">
         <v>3.81</v>
       </c>
-      <c r="J53" s="9">
+      <c r="J53" s="7">
         <v>4.74</v>
       </c>
-      <c r="K53" s="9">
+      <c r="K53" s="7">
         <v>5.55</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="8" t="s">
+      <c r="A54" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B54" s="9">
+      <c r="B54" s="7">
         <v>7.77</v>
       </c>
-      <c r="C54" s="9">
+      <c r="C54" s="7">
         <v>3.27</v>
       </c>
-      <c r="D54" s="9">
+      <c r="D54" s="7">
         <v>2.74</v>
       </c>
-      <c r="E54" s="9">
+      <c r="E54" s="7">
         <v>2.77</v>
       </c>
-      <c r="F54" s="9">
+      <c r="F54" s="7">
         <v>2.9</v>
       </c>
-      <c r="G54" s="9">
+      <c r="G54" s="7">
         <v>3.08</v>
       </c>
-      <c r="H54" s="9">
+      <c r="H54" s="7">
         <v>3.4</v>
       </c>
-      <c r="I54" s="9">
+      <c r="I54" s="7">
         <v>3.61</v>
       </c>
-      <c r="J54" s="9">
+      <c r="J54" s="7">
         <v>4.1900000000000004</v>
       </c>
-      <c r="K54" s="9">
+      <c r="K54" s="7">
         <v>5.03</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="8" t="s">
+      <c r="A55" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B55" s="9">
+      <c r="B55" s="7">
         <v>7.59</v>
       </c>
-      <c r="C55" s="9">
+      <c r="C55" s="7">
         <v>3.16</v>
       </c>
-      <c r="D55" s="9">
+      <c r="D55" s="7">
         <v>2.56</v>
       </c>
-      <c r="E55" s="9">
+      <c r="E55" s="7">
         <v>2.44</v>
       </c>
-      <c r="F55" s="9">
+      <c r="F55" s="7">
         <v>2.37</v>
       </c>
-      <c r="G55" s="9">
+      <c r="G55" s="7">
         <v>2.87</v>
       </c>
-      <c r="H55" s="9">
+      <c r="H55" s="7">
         <v>3.13</v>
       </c>
-      <c r="I55" s="9">
+      <c r="I55" s="7">
         <v>3.75</v>
       </c>
-      <c r="J55" s="9">
+      <c r="J55" s="7">
         <v>3.82</v>
       </c>
-      <c r="K55" s="9">
+      <c r="K55" s="7">
         <v>4.3600000000000003</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="8" t="s">
+      <c r="A56" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B56" s="9">
+      <c r="B56" s="7">
         <v>7.61</v>
       </c>
-      <c r="C56" s="9">
+      <c r="C56" s="7">
         <v>3.28</v>
       </c>
-      <c r="D56" s="9">
+      <c r="D56" s="7">
         <v>2.65</v>
       </c>
-      <c r="E56" s="9">
+      <c r="E56" s="7">
         <v>2.4</v>
       </c>
-      <c r="F56" s="9">
+      <c r="F56" s="7">
         <v>2.7</v>
       </c>
-      <c r="G56" s="9">
+      <c r="G56" s="7">
         <v>2.78</v>
       </c>
-      <c r="H56" s="9">
+      <c r="H56" s="7">
         <v>3.14</v>
       </c>
-      <c r="I56" s="9">
+      <c r="I56" s="7">
         <v>3.57</v>
       </c>
-      <c r="J56" s="9">
+      <c r="J56" s="7">
         <v>3.88</v>
       </c>
-      <c r="K56" s="9">
+      <c r="K56" s="7">
         <v>4.17</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="8" t="s">
+      <c r="A57" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B57" s="9">
+      <c r="B57" s="7">
         <v>7.27</v>
       </c>
-      <c r="C57" s="9">
+      <c r="C57" s="7">
         <v>2.99</v>
       </c>
-      <c r="D57" s="9">
+      <c r="D57" s="7">
         <v>2.41</v>
       </c>
-      <c r="E57" s="9">
+      <c r="E57" s="7">
         <v>2.23</v>
       </c>
-      <c r="F57" s="9">
+      <c r="F57" s="7">
         <v>2.4</v>
       </c>
-      <c r="G57" s="9">
+      <c r="G57" s="7">
         <v>2.63</v>
       </c>
-      <c r="H57" s="9">
+      <c r="H57" s="7">
         <v>2.62</v>
       </c>
-      <c r="I57" s="9">
+      <c r="I57" s="7">
         <v>3.39</v>
       </c>
-      <c r="J57" s="9">
+      <c r="J57" s="7">
         <v>3.99</v>
       </c>
-      <c r="K57" s="9">
+      <c r="K57" s="7">
         <v>4.16</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="8" t="s">
+      <c r="A58" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B58" s="9">
+      <c r="B58" s="7">
         <v>6.84</v>
       </c>
-      <c r="C58" s="9">
+      <c r="C58" s="7">
         <v>3.18</v>
       </c>
-      <c r="D58" s="9">
+      <c r="D58" s="7">
         <v>2.5099999999999998</v>
       </c>
-      <c r="E58" s="9">
+      <c r="E58" s="7">
         <v>2.23</v>
       </c>
-      <c r="F58" s="9">
+      <c r="F58" s="7">
         <v>2.41</v>
       </c>
-      <c r="G58" s="9">
+      <c r="G58" s="7">
         <v>3</v>
       </c>
-      <c r="H58" s="9">
+      <c r="H58" s="7">
         <v>2.83</v>
       </c>
-      <c r="I58" s="9">
+      <c r="I58" s="7">
         <v>3.14</v>
       </c>
-      <c r="J58" s="9">
+      <c r="J58" s="7">
         <v>3.39</v>
       </c>
-      <c r="K58" s="9">
+      <c r="K58" s="7">
         <v>3.76</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="8" t="s">
+      <c r="A59" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B59" s="9">
+      <c r="B59" s="7">
         <v>6.85</v>
       </c>
-      <c r="C59" s="9">
+      <c r="C59" s="7">
         <v>3</v>
       </c>
-      <c r="D59" s="9">
+      <c r="D59" s="7">
         <v>2.52</v>
       </c>
-      <c r="E59" s="9">
+      <c r="E59" s="7">
         <v>2.38</v>
       </c>
-      <c r="F59" s="9">
+      <c r="F59" s="7">
         <v>2.67</v>
       </c>
-      <c r="G59" s="9">
+      <c r="G59" s="7">
         <v>2.93</v>
       </c>
-      <c r="H59" s="9">
+      <c r="H59" s="7">
         <v>3.18</v>
       </c>
-      <c r="I59" s="9">
+      <c r="I59" s="7">
         <v>3.08</v>
       </c>
-      <c r="J59" s="9">
+      <c r="J59" s="7">
         <v>3.57</v>
       </c>
-      <c r="K59" s="9">
+      <c r="K59" s="7">
         <v>3.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix Report 1 and add IC table
</commit_message>
<xml_diff>
--- a/Practica 1. Mixturas de Gaussianas/resultados.xlsx
+++ b/Practica 1. Mixturas de Gaussianas/resultados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel\Nextcloud\ETSINF\2019-20\APR\Practicas\Practica 1. Mixturas de Gaussianas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{590A7F4F-C0B3-4443-8548-5C67C38FF188}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081E3D25-98D4-4583-8E78-3E81E9E6D25F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="27300" windowHeight="15960" activeTab="2" xr2:uid="{70A85A1C-AA30-458D-A4B6-11A0960EF6D5}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet3" sheetId="4" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet1 (2)" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="31">
   <si>
     <t>PCA 10</t>
   </si>
@@ -125,6 +126,9 @@
   </si>
   <si>
     <t>k=1</t>
+  </si>
+  <si>
+    <t>IC 95%</t>
   </si>
 </sst>
 </file>
@@ -244,7 +248,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -276,10 +280,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -287,6 +291,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3784,6 +3794,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$B$2:$B$11</c:f>
@@ -3868,6 +3898,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$C$2:$C$11</c:f>
@@ -3952,6 +4002,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$D$2:$D$11</c:f>
@@ -4036,6 +4106,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$E$2:$E$11</c:f>
@@ -4120,6 +4210,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$F$2:$F$11</c:f>
@@ -4204,6 +4314,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$G$2:$G$11</c:f>
@@ -4294,6 +4424,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$H$2:$H$11</c:f>
@@ -4384,6 +4534,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$I$2:$I$11</c:f>
@@ -4474,6 +4644,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$J$2:$J$11</c:f>
@@ -4564,6 +4754,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$K$2:$K$11</c:f>
@@ -5056,6 +5266,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$B$14:$B$23</c:f>
@@ -5140,6 +5370,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$C$14:$C$23</c:f>
@@ -5224,6 +5474,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$D$14:$D$23</c:f>
@@ -5308,6 +5578,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$E$14:$E$23</c:f>
@@ -5392,6 +5682,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$F$14:$F$23</c:f>
@@ -5476,6 +5786,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$G$14:$G$23</c:f>
@@ -5566,6 +5896,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$H$14:$H$23</c:f>
@@ -5656,6 +6006,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$I$14:$I$23</c:f>
@@ -5746,6 +6116,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$J$14:$J$23</c:f>
@@ -5836,6 +6226,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$K$14:$K$23</c:f>
@@ -6328,6 +6738,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$B$26:$B$35</c:f>
@@ -6412,6 +6842,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$C$26:$C$35</c:f>
@@ -6496,6 +6946,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$D$26:$D$35</c:f>
@@ -6580,6 +7050,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$E$26:$E$35</c:f>
@@ -6664,6 +7154,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$F$26:$F$35</c:f>
@@ -6748,6 +7258,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$G$26:$G$35</c:f>
@@ -6838,6 +7368,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$H$26:$H$35</c:f>
@@ -6928,6 +7478,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$I$26:$I$35</c:f>
@@ -7018,6 +7588,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$J$26:$J$35</c:f>
@@ -7108,6 +7698,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$K$26:$K$35</c:f>
@@ -7600,6 +8210,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$B$38:$B$47</c:f>
@@ -7684,6 +8314,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$C$38:$C$47</c:f>
@@ -7768,6 +8418,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$D$38:$D$47</c:f>
@@ -7852,6 +8522,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$E$38:$E$47</c:f>
@@ -7936,6 +8626,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$F$38:$F$47</c:f>
@@ -8020,6 +8730,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$G$38:$G$47</c:f>
@@ -8110,6 +8840,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$H$38:$H$47</c:f>
@@ -8200,6 +8950,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$I$38:$I$47</c:f>
@@ -8290,6 +9060,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$J$38:$J$47</c:f>
@@ -8380,6 +9170,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$K$38:$K$47</c:f>
@@ -8872,6 +9682,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$B$50:$B$59</c:f>
@@ -8956,6 +9786,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$C$50:$C$59</c:f>
@@ -9040,6 +9890,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$D$50:$D$59</c:f>
@@ -9124,6 +9994,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$E$50:$E$59</c:f>
@@ -9208,6 +10098,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$F$50:$F$59</c:f>
@@ -9292,6 +10202,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$G$50:$G$59</c:f>
@@ -9382,6 +10312,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$H$50:$H$59</c:f>
@@ -9472,6 +10422,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$I$50:$I$59</c:f>
@@ -9562,6 +10532,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$J$50:$J$59</c:f>
@@ -9652,6 +10642,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>'Sheet1 (2)'!$K$50:$K$59</c:f>
@@ -14983,7 +15993,7 @@
   <dimension ref="A1:AI12"/>
   <sheetViews>
     <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="AA3" sqref="AA3"/>
+      <selection activeCell="AA4" sqref="AA4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15002,10 +16012,10 @@
       <c r="C1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="12"/>
+      <c r="N1" s="11"/>
       <c r="O1" s="13" t="s">
         <v>28</v>
       </c>
@@ -15017,10 +16027,10 @@
       <c r="U1" s="14"/>
       <c r="V1" s="14"/>
       <c r="W1" s="14"/>
-      <c r="Y1" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z1" s="12"/>
+      <c r="Y1" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z1" s="11"/>
       <c r="AA1" s="13" t="s">
         <v>28</v>
       </c>
@@ -15044,8 +16054,8 @@
         <f>"±"&amp;TEXT(100*(1.96*SQRT((B2/100)*(1-(B2/100))/60000)),"0.0000")&amp;"%"</f>
         <v>±0.2486%</v>
       </c>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
       <c r="O2" s="1">
         <v>1E-3</v>
       </c>
@@ -15073,8 +16083,8 @@
       <c r="W2" s="1">
         <v>1</v>
       </c>
-      <c r="Y2" s="12"/>
-      <c r="Z2" s="12"/>
+      <c r="Y2" s="11"/>
+      <c r="Z2" s="11"/>
       <c r="AA2" s="1">
         <v>1E-3</v>
       </c>
@@ -15114,7 +16124,7 @@
         <f t="shared" ref="C3:C11" si="0">"±"&amp;TEXT(100*(1.96*SQRT((B3/100)*(1-(B3/100))/60000)),"0.0000")&amp;"%"</f>
         <v>±0.1737%</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="M3" s="12" t="s">
         <v>25</v>
       </c>
       <c r="N3" s="1">
@@ -15147,15 +16157,15 @@
       <c r="W3" s="2">
         <v>10.82</v>
       </c>
-      <c r="Y3" s="11" t="s">
+      <c r="Y3" s="12" t="s">
         <v>25</v>
       </c>
       <c r="Z3" s="1">
         <v>10</v>
       </c>
-      <c r="AA3" s="2" t="str">
-        <f>"±"&amp;TEXT(100*(1.96*SQRT((O3/100)*(1-(O3/100))/60000)),"0.0000")&amp;"%"</f>
-        <v>±0.2579%</v>
+      <c r="AA3" s="2" t="e">
+        <f>Sheet1!B2="±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B2/100)*(1-(Sheet1!B2/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>#VALUE!</v>
       </c>
       <c r="AB3" s="2" t="str">
         <f t="shared" ref="AB3:AI12" si="1">"±"&amp;TEXT(100*(1.96*SQRT((P3/100)*(1-(P3/100))/60000)),"0.0000")&amp;"%"</f>
@@ -15201,7 +16211,7 @@
         <f t="shared" si="0"/>
         <v>±0.1551%</v>
       </c>
-      <c r="M4" s="11"/>
+      <c r="M4" s="12"/>
       <c r="N4" s="1">
         <v>20</v>
       </c>
@@ -15232,7 +16242,7 @@
       <c r="W4" s="2">
         <v>4.96</v>
       </c>
-      <c r="Y4" s="11"/>
+      <c r="Y4" s="12"/>
       <c r="Z4" s="1">
         <v>20</v>
       </c>
@@ -15284,7 +16294,7 @@
         <f t="shared" si="0"/>
         <v>±0.1520%</v>
       </c>
-      <c r="M5" s="11"/>
+      <c r="M5" s="12"/>
       <c r="N5" s="1">
         <v>30</v>
       </c>
@@ -15315,7 +16325,7 @@
       <c r="W5" s="2">
         <v>3.91</v>
       </c>
-      <c r="Y5" s="11"/>
+      <c r="Y5" s="12"/>
       <c r="Z5" s="1">
         <v>30</v>
       </c>
@@ -15367,7 +16377,7 @@
         <f t="shared" si="0"/>
         <v>±0.1499%</v>
       </c>
-      <c r="M6" s="11"/>
+      <c r="M6" s="12"/>
       <c r="N6" s="1">
         <v>40</v>
       </c>
@@ -15398,7 +16408,7 @@
       <c r="W6" s="2">
         <v>3.75</v>
       </c>
-      <c r="Y6" s="11"/>
+      <c r="Y6" s="12"/>
       <c r="Z6" s="1">
         <v>40</v>
       </c>
@@ -15450,7 +16460,7 @@
         <f t="shared" si="0"/>
         <v>±0.1545%</v>
       </c>
-      <c r="M7" s="11"/>
+      <c r="M7" s="12"/>
       <c r="N7" s="1">
         <v>50</v>
       </c>
@@ -15481,7 +16491,7 @@
       <c r="W7" s="2">
         <v>3.64</v>
       </c>
-      <c r="Y7" s="11"/>
+      <c r="Y7" s="12"/>
       <c r="Z7" s="1">
         <v>50</v>
       </c>
@@ -15533,7 +16543,7 @@
         <f t="shared" si="0"/>
         <v>±0.1540%</v>
       </c>
-      <c r="M8" s="11"/>
+      <c r="M8" s="12"/>
       <c r="N8" s="1">
         <v>60</v>
       </c>
@@ -15564,7 +16574,7 @@
       <c r="W8" s="2">
         <v>3.88</v>
       </c>
-      <c r="Y8" s="11"/>
+      <c r="Y8" s="12"/>
       <c r="Z8" s="1">
         <v>60</v>
       </c>
@@ -15616,7 +16626,7 @@
         <f t="shared" si="0"/>
         <v>±0.1568%</v>
       </c>
-      <c r="M9" s="11"/>
+      <c r="M9" s="12"/>
       <c r="N9" s="1">
         <v>70</v>
       </c>
@@ -15647,7 +16657,7 @@
       <c r="W9" s="2">
         <v>3.85</v>
       </c>
-      <c r="Y9" s="11"/>
+      <c r="Y9" s="12"/>
       <c r="Z9" s="1">
         <v>70</v>
       </c>
@@ -15699,7 +16709,7 @@
         <f t="shared" si="0"/>
         <v>±0.1587%</v>
       </c>
-      <c r="M10" s="11"/>
+      <c r="M10" s="12"/>
       <c r="N10" s="1">
         <v>80</v>
       </c>
@@ -15730,7 +16740,7 @@
       <c r="W10" s="2">
         <v>4</v>
       </c>
-      <c r="Y10" s="11"/>
+      <c r="Y10" s="12"/>
       <c r="Z10" s="1">
         <v>80</v>
       </c>
@@ -15782,7 +16792,7 @@
         <f t="shared" si="0"/>
         <v>±0.1623%</v>
       </c>
-      <c r="M11" s="11"/>
+      <c r="M11" s="12"/>
       <c r="N11" s="1">
         <v>90</v>
       </c>
@@ -15813,7 +16823,7 @@
       <c r="W11" s="2">
         <v>4.0999999999999996</v>
       </c>
-      <c r="Y11" s="11"/>
+      <c r="Y11" s="12"/>
       <c r="Z11" s="1">
         <v>90</v>
       </c>
@@ -15855,7 +16865,7 @@
       </c>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="M12" s="11"/>
+      <c r="M12" s="12"/>
       <c r="N12" s="1">
         <v>100</v>
       </c>
@@ -15886,7 +16896,7 @@
       <c r="W12" s="2">
         <v>4.3</v>
       </c>
-      <c r="Y12" s="11"/>
+      <c r="Y12" s="12"/>
       <c r="Z12" s="1">
         <v>100</v>
       </c>
@@ -15982,8 +16992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA25D73-65AF-4565-8849-CEF94185751C}">
   <dimension ref="A1:W6"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="W6" sqref="M1:W6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O18" sqref="O18:P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16094,44 +17104,44 @@
         <v>20</v>
       </c>
       <c r="N2" s="6" t="str">
-        <f>"±"&amp;TEXT(100*(1.96*SQRT((B3/100)*(1-(B3/100))/60000)),"0.0000")&amp;"%"</f>
-        <v>±0.2487%</v>
+        <f>"±"&amp;TEXT(100*(1.96*SQRT((B2/100)*(1-(B2/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2501%</v>
       </c>
       <c r="O2" s="6" t="str">
-        <f t="shared" ref="O2:W2" si="0">"±"&amp;TEXT(100*(1.96*SQRT((C3/100)*(1-(C3/100))/60000)),"0.0000")&amp;"%"</f>
-        <v>±0.1755%</v>
+        <f t="shared" ref="O2:W6" si="0">"±"&amp;TEXT(100*(1.96*SQRT((C2/100)*(1-(C2/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1786%</v>
       </c>
       <c r="P2" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>±0.1598%</v>
+        <v>±0.1661%</v>
       </c>
       <c r="Q2" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>±0.1577%</v>
+        <v>±0.1643%</v>
       </c>
       <c r="R2" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>±0.1560%</v>
+        <v>±0.1630%</v>
       </c>
       <c r="S2" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>±0.1612%</v>
+        <v>±0.1683%</v>
       </c>
       <c r="T2" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>±0.1607%</v>
+        <v>±0.1674%</v>
       </c>
       <c r="U2" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>±0.1646%</v>
+        <v>±0.1714%</v>
       </c>
       <c r="V2" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>±0.1650%</v>
+        <v>±0.1722%</v>
       </c>
       <c r="W2" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>±0.1690%</v>
+        <v>±0.1741%</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
@@ -16172,44 +17182,44 @@
         <v>21</v>
       </c>
       <c r="N3" s="6" t="str">
-        <f t="shared" ref="N3:N6" si="1">"±"&amp;TEXT(100*(1.96*SQRT((B4/100)*(1-(B4/100))/60000)),"0.0000")&amp;"%"</f>
-        <v>±0.2486%</v>
+        <f t="shared" ref="N3:N6" si="1">"±"&amp;TEXT(100*(1.96*SQRT((B3/100)*(1-(B3/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2487%</v>
       </c>
       <c r="O3" s="6" t="str">
-        <f t="shared" ref="O3:O6" si="2">"±"&amp;TEXT(100*(1.96*SQRT((C4/100)*(1-(C4/100))/60000)),"0.0000")&amp;"%"</f>
-        <v>±0.1739%</v>
+        <f t="shared" si="0"/>
+        <v>±0.1755%</v>
       </c>
       <c r="P3" s="6" t="str">
-        <f t="shared" ref="P3:P6" si="3">"±"&amp;TEXT(100*(1.96*SQRT((D4/100)*(1-(D4/100))/60000)),"0.0000")&amp;"%"</f>
-        <v>±0.1566%</v>
+        <f t="shared" si="0"/>
+        <v>±0.1598%</v>
       </c>
       <c r="Q3" s="6" t="str">
-        <f t="shared" ref="Q3:Q6" si="4">"±"&amp;TEXT(100*(1.96*SQRT((E4/100)*(1-(E4/100))/60000)),"0.0000")&amp;"%"</f>
-        <v>±0.1540%</v>
+        <f t="shared" si="0"/>
+        <v>±0.1577%</v>
       </c>
       <c r="R3" s="6" t="str">
-        <f t="shared" ref="R3:R6" si="5">"±"&amp;TEXT(100*(1.96*SQRT((F4/100)*(1-(F4/100))/60000)),"0.0000")&amp;"%"</f>
-        <v>±0.1510%</v>
+        <f t="shared" si="0"/>
+        <v>±0.1560%</v>
       </c>
       <c r="S3" s="6" t="str">
-        <f t="shared" ref="S3:S6" si="6">"±"&amp;TEXT(100*(1.96*SQRT((G4/100)*(1-(G4/100))/60000)),"0.0000")&amp;"%"</f>
-        <v>±0.1559%</v>
+        <f t="shared" si="0"/>
+        <v>±0.1612%</v>
       </c>
       <c r="T3" s="6" t="str">
-        <f t="shared" ref="T3:T6" si="7">"±"&amp;TEXT(100*(1.96*SQRT((H4/100)*(1-(H4/100))/60000)),"0.0000")&amp;"%"</f>
-        <v>±0.1553%</v>
+        <f t="shared" si="0"/>
+        <v>±0.1607%</v>
       </c>
       <c r="U3" s="6" t="str">
-        <f t="shared" ref="U3:U6" si="8">"±"&amp;TEXT(100*(1.96*SQRT((I4/100)*(1-(I4/100))/60000)),"0.0000")&amp;"%"</f>
-        <v>±0.1587%</v>
+        <f t="shared" si="0"/>
+        <v>±0.1646%</v>
       </c>
       <c r="V3" s="6" t="str">
-        <f t="shared" ref="V3:V6" si="9">"±"&amp;TEXT(100*(1.96*SQRT((J4/100)*(1-(J4/100))/60000)),"0.0000")&amp;"%"</f>
-        <v>±0.1590%</v>
+        <f t="shared" si="0"/>
+        <v>±0.1650%</v>
       </c>
       <c r="W3" s="6" t="str">
-        <f t="shared" ref="W3:W6" si="10">"±"&amp;TEXT(100*(1.96*SQRT((K4/100)*(1-(K4/100))/60000)),"0.0000")&amp;"%"</f>
-        <v>±0.1645%</v>
+        <f t="shared" si="0"/>
+        <v>±0.1690%</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
@@ -16254,40 +17264,40 @@
         <v>±0.2486%</v>
       </c>
       <c r="O4" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>±0.1741%</v>
+        <f t="shared" si="0"/>
+        <v>±0.1739%</v>
       </c>
       <c r="P4" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>±0.1566%</v>
       </c>
       <c r="Q4" s="6" t="str">
-        <f t="shared" si="4"/>
-        <v>±0.1526%</v>
+        <f t="shared" si="0"/>
+        <v>±0.1540%</v>
       </c>
       <c r="R4" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>±0.1510%</v>
       </c>
       <c r="S4" s="6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
+        <v>±0.1559%</v>
+      </c>
+      <c r="T4" s="6" t="str">
+        <f t="shared" si="0"/>
         <v>±0.1553%</v>
       </c>
-      <c r="T4" s="6" t="str">
-        <f t="shared" si="7"/>
-        <v>±0.1545%</v>
-      </c>
       <c r="U4" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v>±0.1574%</v>
+        <f t="shared" si="0"/>
+        <v>±0.1587%</v>
       </c>
       <c r="V4" s="6" t="str">
-        <f t="shared" si="9"/>
-        <v>±0.1581%</v>
+        <f t="shared" si="0"/>
+        <v>±0.1590%</v>
       </c>
       <c r="W4" s="6" t="str">
-        <f t="shared" si="10"/>
-        <v>±0.1630%</v>
+        <f t="shared" si="0"/>
+        <v>±0.1645%</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
@@ -16329,43 +17339,43 @@
       </c>
       <c r="N5" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>±0.2485%</v>
+        <v>±0.2486%</v>
       </c>
       <c r="O5" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>±0.1741%</v>
       </c>
       <c r="P5" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
+        <v>±0.1566%</v>
+      </c>
+      <c r="Q5" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>±0.1526%</v>
+      </c>
+      <c r="R5" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>±0.1510%</v>
+      </c>
+      <c r="S5" s="6" t="str">
+        <f t="shared" si="0"/>
         <v>±0.1553%</v>
       </c>
-      <c r="Q5" s="6" t="str">
-        <f t="shared" si="4"/>
-        <v>±0.1524%</v>
-      </c>
-      <c r="R5" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v>±0.1497%</v>
-      </c>
-      <c r="S5" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>±0.1549%</v>
-      </c>
       <c r="T5" s="6" t="str">
-        <f t="shared" si="7"/>
-        <v>±0.1541%</v>
+        <f t="shared" si="0"/>
+        <v>±0.1545%</v>
       </c>
       <c r="U5" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v>±0.1566%</v>
+        <f t="shared" si="0"/>
+        <v>±0.1574%</v>
       </c>
       <c r="V5" s="6" t="str">
-        <f t="shared" si="9"/>
-        <v>±0.1585%</v>
+        <f t="shared" si="0"/>
+        <v>±0.1581%</v>
       </c>
       <c r="W5" s="6" t="str">
-        <f t="shared" si="10"/>
-        <v>±0.1621%</v>
+        <f t="shared" si="0"/>
+        <v>±0.1630%</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
@@ -16407,43 +17417,43 @@
       </c>
       <c r="N6" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>±0.0000%</v>
+        <v>±0.2485%</v>
       </c>
       <c r="O6" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>±0.0000%</v>
+        <f t="shared" si="0"/>
+        <v>±0.1741%</v>
       </c>
       <c r="P6" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v>±0.0000%</v>
+        <f t="shared" si="0"/>
+        <v>±0.1553%</v>
       </c>
       <c r="Q6" s="6" t="str">
-        <f t="shared" si="4"/>
-        <v>±0.0000%</v>
+        <f t="shared" si="0"/>
+        <v>±0.1524%</v>
       </c>
       <c r="R6" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v>±0.0000%</v>
+        <f t="shared" si="0"/>
+        <v>±0.1497%</v>
       </c>
       <c r="S6" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>±0.0000%</v>
+        <f t="shared" si="0"/>
+        <v>±0.1549%</v>
       </c>
       <c r="T6" s="6" t="str">
-        <f t="shared" si="7"/>
-        <v>±0.0000%</v>
+        <f t="shared" si="0"/>
+        <v>±0.1541%</v>
       </c>
       <c r="U6" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v>±0.0000%</v>
+        <f t="shared" si="0"/>
+        <v>±0.1566%</v>
       </c>
       <c r="V6" s="6" t="str">
-        <f t="shared" si="9"/>
-        <v>±0.0000%</v>
+        <f t="shared" si="0"/>
+        <v>±0.1585%</v>
       </c>
       <c r="W6" s="6" t="str">
-        <f t="shared" si="10"/>
-        <v>±0.0000%</v>
+        <f t="shared" si="0"/>
+        <v>±0.1621%</v>
       </c>
     </row>
   </sheetData>
@@ -16480,8 +17490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E91C0581-E8C2-4506-9305-1F1CBC86D7DE}">
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="K59" sqref="A1:K59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18486,4 +19496,2496 @@
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCEE6135-78AC-47B6-B5FF-AA86191398DE}">
+  <dimension ref="A1:K59"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K59" sqref="A1:K59"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B2/100)*(1-('Sheet1 (2)'!B2/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2501%</v>
+      </c>
+      <c r="C2" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C2/100)*(1-('Sheet1 (2)'!C2/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1786%</v>
+      </c>
+      <c r="D2" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D2/100)*(1-('Sheet1 (2)'!D2/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1661%</v>
+      </c>
+      <c r="E2" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E2/100)*(1-('Sheet1 (2)'!E2/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1643%</v>
+      </c>
+      <c r="F2" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F2/100)*(1-('Sheet1 (2)'!F2/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1630%</v>
+      </c>
+      <c r="G2" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G2/100)*(1-('Sheet1 (2)'!G2/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1683%</v>
+      </c>
+      <c r="H2" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H2/100)*(1-('Sheet1 (2)'!H2/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1674%</v>
+      </c>
+      <c r="I2" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I2/100)*(1-('Sheet1 (2)'!I2/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1714%</v>
+      </c>
+      <c r="J2" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J2/100)*(1-('Sheet1 (2)'!J2/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1722%</v>
+      </c>
+      <c r="K2" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K2/100)*(1-('Sheet1 (2)'!K2/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1741%</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B3/100)*(1-('Sheet1 (2)'!B3/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2426%</v>
+      </c>
+      <c r="C3" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C3/100)*(1-('Sheet1 (2)'!C3/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1710%</v>
+      </c>
+      <c r="D3" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D3/100)*(1-('Sheet1 (2)'!D3/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1566%</v>
+      </c>
+      <c r="E3" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E3/100)*(1-('Sheet1 (2)'!E3/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1585%</v>
+      </c>
+      <c r="F3" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F3/100)*(1-('Sheet1 (2)'!F3/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1547%</v>
+      </c>
+      <c r="G3" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G3/100)*(1-('Sheet1 (2)'!G3/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1583%</v>
+      </c>
+      <c r="H3" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H3/100)*(1-('Sheet1 (2)'!H3/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1590%</v>
+      </c>
+      <c r="I3" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I3/100)*(1-('Sheet1 (2)'!I3/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1636%</v>
+      </c>
+      <c r="J3" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J3/100)*(1-('Sheet1 (2)'!J3/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1727%</v>
+      </c>
+      <c r="K3" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K3/100)*(1-('Sheet1 (2)'!K3/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1812%</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B4/100)*(1-('Sheet1 (2)'!B4/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2306%</v>
+      </c>
+      <c r="C4" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C4/100)*(1-('Sheet1 (2)'!C4/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1685%</v>
+      </c>
+      <c r="D4" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D4/100)*(1-('Sheet1 (2)'!D4/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1487%</v>
+      </c>
+      <c r="E4" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E4/100)*(1-('Sheet1 (2)'!E4/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1499%</v>
+      </c>
+      <c r="F4" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F4/100)*(1-('Sheet1 (2)'!F4/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1491%</v>
+      </c>
+      <c r="G4" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G4/100)*(1-('Sheet1 (2)'!G4/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1607%</v>
+      </c>
+      <c r="H4" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H4/100)*(1-('Sheet1 (2)'!H4/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1625%</v>
+      </c>
+      <c r="I4" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I4/100)*(1-('Sheet1 (2)'!I4/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1697%</v>
+      </c>
+      <c r="J4" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J4/100)*(1-('Sheet1 (2)'!J4/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1716%</v>
+      </c>
+      <c r="K4" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K4/100)*(1-('Sheet1 (2)'!K4/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1741%</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B5/100)*(1-('Sheet1 (2)'!B5/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2324%</v>
+      </c>
+      <c r="C5" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C5/100)*(1-('Sheet1 (2)'!C5/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1590%</v>
+      </c>
+      <c r="D5" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D5/100)*(1-('Sheet1 (2)'!D5/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1598%</v>
+      </c>
+      <c r="E5" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E5/100)*(1-('Sheet1 (2)'!E5/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1487%</v>
+      </c>
+      <c r="F5" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F5/100)*(1-('Sheet1 (2)'!F5/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1518%</v>
+      </c>
+      <c r="G5" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G5/100)*(1-('Sheet1 (2)'!G5/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1603%</v>
+      </c>
+      <c r="H5" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H5/100)*(1-('Sheet1 (2)'!H5/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1559%</v>
+      </c>
+      <c r="I5" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I5/100)*(1-('Sheet1 (2)'!I5/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1630%</v>
+      </c>
+      <c r="J5" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J5/100)*(1-('Sheet1 (2)'!J5/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1717%</v>
+      </c>
+      <c r="K5" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K5/100)*(1-('Sheet1 (2)'!K5/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1799%</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B6/100)*(1-('Sheet1 (2)'!B6/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2324%</v>
+      </c>
+      <c r="C6" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C6/100)*(1-('Sheet1 (2)'!C6/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1532%</v>
+      </c>
+      <c r="D6" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D6/100)*(1-('Sheet1 (2)'!D6/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1506%</v>
+      </c>
+      <c r="E6" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E6/100)*(1-('Sheet1 (2)'!E6/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1425%</v>
+      </c>
+      <c r="F6" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F6/100)*(1-('Sheet1 (2)'!F6/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1456%</v>
+      </c>
+      <c r="G6" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G6/100)*(1-('Sheet1 (2)'!G6/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1481%</v>
+      </c>
+      <c r="H6" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H6/100)*(1-('Sheet1 (2)'!H6/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1598%</v>
+      </c>
+      <c r="I6" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I6/100)*(1-('Sheet1 (2)'!I6/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1587%</v>
+      </c>
+      <c r="J6" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J6/100)*(1-('Sheet1 (2)'!J6/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1668%</v>
+      </c>
+      <c r="K6" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K6/100)*(1-('Sheet1 (2)'!K6/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1727%</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B7/100)*(1-('Sheet1 (2)'!B7/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2269%</v>
+      </c>
+      <c r="C7" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C7/100)*(1-('Sheet1 (2)'!C7/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1620%</v>
+      </c>
+      <c r="D7" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D7/100)*(1-('Sheet1 (2)'!D7/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1404%</v>
+      </c>
+      <c r="E7" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E7/100)*(1-('Sheet1 (2)'!E7/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1406%</v>
+      </c>
+      <c r="F7" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F7/100)*(1-('Sheet1 (2)'!F7/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1329%</v>
+      </c>
+      <c r="G7" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G7/100)*(1-('Sheet1 (2)'!G7/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1454%</v>
+      </c>
+      <c r="H7" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H7/100)*(1-('Sheet1 (2)'!H7/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1524%</v>
+      </c>
+      <c r="I7" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I7/100)*(1-('Sheet1 (2)'!I7/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1551%</v>
+      </c>
+      <c r="J7" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J7/100)*(1-('Sheet1 (2)'!J7/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1607%</v>
+      </c>
+      <c r="K7" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K7/100)*(1-('Sheet1 (2)'!K7/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1700%</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B8/100)*(1-('Sheet1 (2)'!B8/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2281%</v>
+      </c>
+      <c r="C8" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C8/100)*(1-('Sheet1 (2)'!C8/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1607%</v>
+      </c>
+      <c r="D8" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D8/100)*(1-('Sheet1 (2)'!D8/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1479%</v>
+      </c>
+      <c r="E8" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E8/100)*(1-('Sheet1 (2)'!E8/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1391%</v>
+      </c>
+      <c r="F8" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F8/100)*(1-('Sheet1 (2)'!F8/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1431%</v>
+      </c>
+      <c r="G8" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G8/100)*(1-('Sheet1 (2)'!G8/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1506%</v>
+      </c>
+      <c r="H8" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H8/100)*(1-('Sheet1 (2)'!H8/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1596%</v>
+      </c>
+      <c r="I8" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I8/100)*(1-('Sheet1 (2)'!I8/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1612%</v>
+      </c>
+      <c r="J8" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J8/100)*(1-('Sheet1 (2)'!J8/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1562%</v>
+      </c>
+      <c r="K8" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K8/100)*(1-('Sheet1 (2)'!K8/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1666%</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B9/100)*(1-('Sheet1 (2)'!B9/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2187%</v>
+      </c>
+      <c r="C9" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C9/100)*(1-('Sheet1 (2)'!C9/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1530%</v>
+      </c>
+      <c r="D9" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D9/100)*(1-('Sheet1 (2)'!D9/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1336%</v>
+      </c>
+      <c r="E9" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E9/100)*(1-('Sheet1 (2)'!E9/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1340%</v>
+      </c>
+      <c r="F9" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F9/100)*(1-('Sheet1 (2)'!F9/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1340%</v>
+      </c>
+      <c r="G9" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G9/100)*(1-('Sheet1 (2)'!G9/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1425%</v>
+      </c>
+      <c r="H9" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H9/100)*(1-('Sheet1 (2)'!H9/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1489%</v>
+      </c>
+      <c r="I9" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I9/100)*(1-('Sheet1 (2)'!I9/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1590%</v>
+      </c>
+      <c r="J9" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J9/100)*(1-('Sheet1 (2)'!J9/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1705%</v>
+      </c>
+      <c r="K9" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K9/100)*(1-('Sheet1 (2)'!K9/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1678%</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B10/100)*(1-('Sheet1 (2)'!B10/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2220%</v>
+      </c>
+      <c r="C10" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C10/100)*(1-('Sheet1 (2)'!C10/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1499%</v>
+      </c>
+      <c r="D10" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D10/100)*(1-('Sheet1 (2)'!D10/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1361%</v>
+      </c>
+      <c r="E10" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E10/100)*(1-('Sheet1 (2)'!E10/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1361%</v>
+      </c>
+      <c r="F10" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F10/100)*(1-('Sheet1 (2)'!F10/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1440%</v>
+      </c>
+      <c r="G10" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G10/100)*(1-('Sheet1 (2)'!G10/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1473%</v>
+      </c>
+      <c r="H10" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H10/100)*(1-('Sheet1 (2)'!H10/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1579%</v>
+      </c>
+      <c r="I10" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I10/100)*(1-('Sheet1 (2)'!I10/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1612%</v>
+      </c>
+      <c r="J10" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J10/100)*(1-('Sheet1 (2)'!J10/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1674%</v>
+      </c>
+      <c r="K10" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K10/100)*(1-('Sheet1 (2)'!K10/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1712%</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B11/100)*(1-('Sheet1 (2)'!B11/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2228%</v>
+      </c>
+      <c r="C11" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C11/100)*(1-('Sheet1 (2)'!C11/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1514%</v>
+      </c>
+      <c r="D11" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D11/100)*(1-('Sheet1 (2)'!D11/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1349%</v>
+      </c>
+      <c r="E11" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E11/100)*(1-('Sheet1 (2)'!E11/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1452%</v>
+      </c>
+      <c r="F11" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F11/100)*(1-('Sheet1 (2)'!F11/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1460%</v>
+      </c>
+      <c r="G11" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G11/100)*(1-('Sheet1 (2)'!G11/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1431%</v>
+      </c>
+      <c r="H11" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H11/100)*(1-('Sheet1 (2)'!H11/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1510%</v>
+      </c>
+      <c r="I11" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I11/100)*(1-('Sheet1 (2)'!I11/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1630%</v>
+      </c>
+      <c r="J11" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J11/100)*(1-('Sheet1 (2)'!J11/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1620%</v>
+      </c>
+      <c r="K11" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K11/100)*(1-('Sheet1 (2)'!K11/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1625%</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B14/100)*(1-('Sheet1 (2)'!B14/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2487%</v>
+      </c>
+      <c r="C14" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C14/100)*(1-('Sheet1 (2)'!C14/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1755%</v>
+      </c>
+      <c r="D14" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D14/100)*(1-('Sheet1 (2)'!D14/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1598%</v>
+      </c>
+      <c r="E14" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E14/100)*(1-('Sheet1 (2)'!E14/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1577%</v>
+      </c>
+      <c r="F14" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F14/100)*(1-('Sheet1 (2)'!F14/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1560%</v>
+      </c>
+      <c r="G14" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G14/100)*(1-('Sheet1 (2)'!G14/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1612%</v>
+      </c>
+      <c r="H14" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H14/100)*(1-('Sheet1 (2)'!H14/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1607%</v>
+      </c>
+      <c r="I14" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I14/100)*(1-('Sheet1 (2)'!I14/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1646%</v>
+      </c>
+      <c r="J14" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J14/100)*(1-('Sheet1 (2)'!J14/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1650%</v>
+      </c>
+      <c r="K14" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K14/100)*(1-('Sheet1 (2)'!K14/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1690%</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B15/100)*(1-('Sheet1 (2)'!B15/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2409%</v>
+      </c>
+      <c r="C15" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C15/100)*(1-('Sheet1 (2)'!C15/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1714%</v>
+      </c>
+      <c r="D15" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D15/100)*(1-('Sheet1 (2)'!D15/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1543%</v>
+      </c>
+      <c r="E15" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E15/100)*(1-('Sheet1 (2)'!E15/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1508%</v>
+      </c>
+      <c r="F15" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F15/100)*(1-('Sheet1 (2)'!F15/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1499%</v>
+      </c>
+      <c r="G15" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G15/100)*(1-('Sheet1 (2)'!G15/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1543%</v>
+      </c>
+      <c r="H15" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H15/100)*(1-('Sheet1 (2)'!H15/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1581%</v>
+      </c>
+      <c r="I15" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I15/100)*(1-('Sheet1 (2)'!I15/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1607%</v>
+      </c>
+      <c r="J15" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J15/100)*(1-('Sheet1 (2)'!J15/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1714%</v>
+      </c>
+      <c r="K15" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K15/100)*(1-('Sheet1 (2)'!K15/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1757%</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B16/100)*(1-('Sheet1 (2)'!B16/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2247%</v>
+      </c>
+      <c r="C16" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C16/100)*(1-('Sheet1 (2)'!C16/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1638%</v>
+      </c>
+      <c r="D16" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D16/100)*(1-('Sheet1 (2)'!D16/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1475%</v>
+      </c>
+      <c r="E16" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E16/100)*(1-('Sheet1 (2)'!E16/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1421%</v>
+      </c>
+      <c r="F16" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F16/100)*(1-('Sheet1 (2)'!F16/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1444%</v>
+      </c>
+      <c r="G16" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G16/100)*(1-('Sheet1 (2)'!G16/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1510%</v>
+      </c>
+      <c r="H16" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H16/100)*(1-('Sheet1 (2)'!H16/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1560%</v>
+      </c>
+      <c r="I16" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I16/100)*(1-('Sheet1 (2)'!I16/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1587%</v>
+      </c>
+      <c r="J16" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J16/100)*(1-('Sheet1 (2)'!J16/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1601%</v>
+      </c>
+      <c r="K16" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K16/100)*(1-('Sheet1 (2)'!K16/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1707%</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B17/100)*(1-('Sheet1 (2)'!B17/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2268%</v>
+      </c>
+      <c r="C17" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C17/100)*(1-('Sheet1 (2)'!C17/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1551%</v>
+      </c>
+      <c r="D17" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D17/100)*(1-('Sheet1 (2)'!D17/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1475%</v>
+      </c>
+      <c r="E17" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E17/100)*(1-('Sheet1 (2)'!E17/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1438%</v>
+      </c>
+      <c r="F17" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F17/100)*(1-('Sheet1 (2)'!F17/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1417%</v>
+      </c>
+      <c r="G17" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G17/100)*(1-('Sheet1 (2)'!G17/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1469%</v>
+      </c>
+      <c r="H17" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H17/100)*(1-('Sheet1 (2)'!H17/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1503%</v>
+      </c>
+      <c r="I17" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I17/100)*(1-('Sheet1 (2)'!I17/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1623%</v>
+      </c>
+      <c r="J17" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J17/100)*(1-('Sheet1 (2)'!J17/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1666%</v>
+      </c>
+      <c r="K17" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K17/100)*(1-('Sheet1 (2)'!K17/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1772%</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B18/100)*(1-('Sheet1 (2)'!B18/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2283%</v>
+      </c>
+      <c r="C18" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C18/100)*(1-('Sheet1 (2)'!C18/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1446%</v>
+      </c>
+      <c r="D18" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D18/100)*(1-('Sheet1 (2)'!D18/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1436%</v>
+      </c>
+      <c r="E18" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E18/100)*(1-('Sheet1 (2)'!E18/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1365%</v>
+      </c>
+      <c r="F18" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F18/100)*(1-('Sheet1 (2)'!F18/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1389%</v>
+      </c>
+      <c r="G18" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G18/100)*(1-('Sheet1 (2)'!G18/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1395%</v>
+      </c>
+      <c r="H18" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H18/100)*(1-('Sheet1 (2)'!H18/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1516%</v>
+      </c>
+      <c r="I18" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I18/100)*(1-('Sheet1 (2)'!I18/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1562%</v>
+      </c>
+      <c r="J18" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J18/100)*(1-('Sheet1 (2)'!J18/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1605%</v>
+      </c>
+      <c r="K18" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K18/100)*(1-('Sheet1 (2)'!K18/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1681%</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B19/100)*(1-('Sheet1 (2)'!B19/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2187%</v>
+      </c>
+      <c r="C19" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C19/100)*(1-('Sheet1 (2)'!C19/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1534%</v>
+      </c>
+      <c r="D19" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D19/100)*(1-('Sheet1 (2)'!D19/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1358%</v>
+      </c>
+      <c r="E19" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E19/100)*(1-('Sheet1 (2)'!E19/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1304%</v>
+      </c>
+      <c r="F19" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F19/100)*(1-('Sheet1 (2)'!F19/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1313%</v>
+      </c>
+      <c r="G19" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G19/100)*(1-('Sheet1 (2)'!G19/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1438%</v>
+      </c>
+      <c r="H19" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H19/100)*(1-('Sheet1 (2)'!H19/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1406%</v>
+      </c>
+      <c r="I19" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I19/100)*(1-('Sheet1 (2)'!I19/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1483%</v>
+      </c>
+      <c r="J19" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J19/100)*(1-('Sheet1 (2)'!J19/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1501%</v>
+      </c>
+      <c r="K19" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K19/100)*(1-('Sheet1 (2)'!K19/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1609%</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B20/100)*(1-('Sheet1 (2)'!B20/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2211%</v>
+      </c>
+      <c r="C20" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C20/100)*(1-('Sheet1 (2)'!C20/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1508%</v>
+      </c>
+      <c r="D20" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D20/100)*(1-('Sheet1 (2)'!D20/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1322%</v>
+      </c>
+      <c r="E20" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E20/100)*(1-('Sheet1 (2)'!E20/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1349%</v>
+      </c>
+      <c r="F20" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F20/100)*(1-('Sheet1 (2)'!F20/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1334%</v>
+      </c>
+      <c r="G20" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G20/100)*(1-('Sheet1 (2)'!G20/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1382%</v>
+      </c>
+      <c r="H20" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H20/100)*(1-('Sheet1 (2)'!H20/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1481%</v>
+      </c>
+      <c r="I20" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I20/100)*(1-('Sheet1 (2)'!I20/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1487%</v>
+      </c>
+      <c r="J20" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J20/100)*(1-('Sheet1 (2)'!J20/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1516%</v>
+      </c>
+      <c r="K20" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K20/100)*(1-('Sheet1 (2)'!K20/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1562%</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B21/100)*(1-('Sheet1 (2)'!B21/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2124%</v>
+      </c>
+      <c r="C21" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C21/100)*(1-('Sheet1 (2)'!C21/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1489%</v>
+      </c>
+      <c r="D21" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D21/100)*(1-('Sheet1 (2)'!D21/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1283%</v>
+      </c>
+      <c r="E21" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E21/100)*(1-('Sheet1 (2)'!E21/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1271%</v>
+      </c>
+      <c r="F21" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F21/100)*(1-('Sheet1 (2)'!F21/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1311%</v>
+      </c>
+      <c r="G21" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G21/100)*(1-('Sheet1 (2)'!G21/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1365%</v>
+      </c>
+      <c r="H21" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H21/100)*(1-('Sheet1 (2)'!H21/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1415%</v>
+      </c>
+      <c r="I21" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I21/100)*(1-('Sheet1 (2)'!I21/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1520%</v>
+      </c>
+      <c r="J21" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J21/100)*(1-('Sheet1 (2)'!J21/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1645%</v>
+      </c>
+      <c r="K21" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K21/100)*(1-('Sheet1 (2)'!K21/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1643%</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B22/100)*(1-('Sheet1 (2)'!B22/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2131%</v>
+      </c>
+      <c r="C22" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C22/100)*(1-('Sheet1 (2)'!C22/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1448%</v>
+      </c>
+      <c r="D22" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D22/100)*(1-('Sheet1 (2)'!D22/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1325%</v>
+      </c>
+      <c r="E22" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E22/100)*(1-('Sheet1 (2)'!E22/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1257%</v>
+      </c>
+      <c r="F22" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F22/100)*(1-('Sheet1 (2)'!F22/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1329%</v>
+      </c>
+      <c r="G22" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G22/100)*(1-('Sheet1 (2)'!G22/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1442%</v>
+      </c>
+      <c r="H22" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H22/100)*(1-('Sheet1 (2)'!H22/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1382%</v>
+      </c>
+      <c r="I22" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I22/100)*(1-('Sheet1 (2)'!I22/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1427%</v>
+      </c>
+      <c r="J22" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J22/100)*(1-('Sheet1 (2)'!J22/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1566%</v>
+      </c>
+      <c r="K22" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K22/100)*(1-('Sheet1 (2)'!K22/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1609%</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B23/100)*(1-('Sheet1 (2)'!B23/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2146%</v>
+      </c>
+      <c r="C23" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C23/100)*(1-('Sheet1 (2)'!C23/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1429%</v>
+      </c>
+      <c r="D23" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D23/100)*(1-('Sheet1 (2)'!D23/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1322%</v>
+      </c>
+      <c r="E23" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E23/100)*(1-('Sheet1 (2)'!E23/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1271%</v>
+      </c>
+      <c r="F23" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F23/100)*(1-('Sheet1 (2)'!F23/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1349%</v>
+      </c>
+      <c r="G23" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G23/100)*(1-('Sheet1 (2)'!G23/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1365%</v>
+      </c>
+      <c r="H23" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H23/100)*(1-('Sheet1 (2)'!H23/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1446%</v>
+      </c>
+      <c r="I23" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I23/100)*(1-('Sheet1 (2)'!I23/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1464%</v>
+      </c>
+      <c r="J23" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J23/100)*(1-('Sheet1 (2)'!J23/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1549%</v>
+      </c>
+      <c r="K23" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K23/100)*(1-('Sheet1 (2)'!K23/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1559%</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="9"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B26/100)*(1-('Sheet1 (2)'!B26/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2486%</v>
+      </c>
+      <c r="C26" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C26/100)*(1-('Sheet1 (2)'!C26/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1739%</v>
+      </c>
+      <c r="D26" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D26/100)*(1-('Sheet1 (2)'!D26/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1566%</v>
+      </c>
+      <c r="E26" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E26/100)*(1-('Sheet1 (2)'!E26/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1540%</v>
+      </c>
+      <c r="F26" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F26/100)*(1-('Sheet1 (2)'!F26/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1510%</v>
+      </c>
+      <c r="G26" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G26/100)*(1-('Sheet1 (2)'!G26/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1559%</v>
+      </c>
+      <c r="H26" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H26/100)*(1-('Sheet1 (2)'!H26/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1553%</v>
+      </c>
+      <c r="I26" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I26/100)*(1-('Sheet1 (2)'!I26/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1587%</v>
+      </c>
+      <c r="J26" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J26/100)*(1-('Sheet1 (2)'!J26/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1590%</v>
+      </c>
+      <c r="K26" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K26/100)*(1-('Sheet1 (2)'!K26/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1645%</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B27/100)*(1-('Sheet1 (2)'!B27/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2368%</v>
+      </c>
+      <c r="C27" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C27/100)*(1-('Sheet1 (2)'!C27/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1681%</v>
+      </c>
+      <c r="D27" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D27/100)*(1-('Sheet1 (2)'!D27/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1514%</v>
+      </c>
+      <c r="E27" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E27/100)*(1-('Sheet1 (2)'!E27/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1438%</v>
+      </c>
+      <c r="F27" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F27/100)*(1-('Sheet1 (2)'!F27/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1462%</v>
+      </c>
+      <c r="G27" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G27/100)*(1-('Sheet1 (2)'!G27/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1499%</v>
+      </c>
+      <c r="H27" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H27/100)*(1-('Sheet1 (2)'!H27/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1566%</v>
+      </c>
+      <c r="I27" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I27/100)*(1-('Sheet1 (2)'!I27/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1587%</v>
+      </c>
+      <c r="J27" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J27/100)*(1-('Sheet1 (2)'!J27/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1739%</v>
+      </c>
+      <c r="K27" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K27/100)*(1-('Sheet1 (2)'!K27/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1773%</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B28/100)*(1-('Sheet1 (2)'!B28/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2246%</v>
+      </c>
+      <c r="C28" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C28/100)*(1-('Sheet1 (2)'!C28/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1620%</v>
+      </c>
+      <c r="D28" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D28/100)*(1-('Sheet1 (2)'!D28/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1429%</v>
+      </c>
+      <c r="E28" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E28/100)*(1-('Sheet1 (2)'!E28/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1358%</v>
+      </c>
+      <c r="F28" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F28/100)*(1-('Sheet1 (2)'!F28/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1415%</v>
+      </c>
+      <c r="G28" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G28/100)*(1-('Sheet1 (2)'!G28/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1446%</v>
+      </c>
+      <c r="H28" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H28/100)*(1-('Sheet1 (2)'!H28/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1501%</v>
+      </c>
+      <c r="I28" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I28/100)*(1-('Sheet1 (2)'!I28/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1518%</v>
+      </c>
+      <c r="J28" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J28/100)*(1-('Sheet1 (2)'!J28/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1579%</v>
+      </c>
+      <c r="K28" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K28/100)*(1-('Sheet1 (2)'!K28/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1717%</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B29/100)*(1-('Sheet1 (2)'!B29/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2253%</v>
+      </c>
+      <c r="C29" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C29/100)*(1-('Sheet1 (2)'!C29/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1505%</v>
+      </c>
+      <c r="D29" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D29/100)*(1-('Sheet1 (2)'!D29/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1423%</v>
+      </c>
+      <c r="E29" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E29/100)*(1-('Sheet1 (2)'!E29/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1365%</v>
+      </c>
+      <c r="F29" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F29/100)*(1-('Sheet1 (2)'!F29/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1378%</v>
+      </c>
+      <c r="G29" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G29/100)*(1-('Sheet1 (2)'!G29/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1448%</v>
+      </c>
+      <c r="H29" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H29/100)*(1-('Sheet1 (2)'!H29/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1473%</v>
+      </c>
+      <c r="I29" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I29/100)*(1-('Sheet1 (2)'!I29/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1540%</v>
+      </c>
+      <c r="J29" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J29/100)*(1-('Sheet1 (2)'!J29/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1657%</v>
+      </c>
+      <c r="K29" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K29/100)*(1-('Sheet1 (2)'!K29/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1830%</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B30/100)*(1-('Sheet1 (2)'!B30/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2176%</v>
+      </c>
+      <c r="C30" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C30/100)*(1-('Sheet1 (2)'!C30/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1458%</v>
+      </c>
+      <c r="D30" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D30/100)*(1-('Sheet1 (2)'!D30/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1354%</v>
+      </c>
+      <c r="E30" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E30/100)*(1-('Sheet1 (2)'!E30/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1345%</v>
+      </c>
+      <c r="F30" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F30/100)*(1-('Sheet1 (2)'!F30/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1331%</v>
+      </c>
+      <c r="G30" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G30/100)*(1-('Sheet1 (2)'!G30/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1378%</v>
+      </c>
+      <c r="H30" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H30/100)*(1-('Sheet1 (2)'!H30/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1444%</v>
+      </c>
+      <c r="I30" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I30/100)*(1-('Sheet1 (2)'!I30/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1512%</v>
+      </c>
+      <c r="J30" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J30/100)*(1-('Sheet1 (2)'!J30/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1607%</v>
+      </c>
+      <c r="K30" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K30/100)*(1-('Sheet1 (2)'!K30/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1716%</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B31/100)*(1-('Sheet1 (2)'!B31/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2131%</v>
+      </c>
+      <c r="C31" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C31/100)*(1-('Sheet1 (2)'!C31/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1491%</v>
+      </c>
+      <c r="D31" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D31/100)*(1-('Sheet1 (2)'!D31/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1288%</v>
+      </c>
+      <c r="E31" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E31/100)*(1-('Sheet1 (2)'!E31/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1249%</v>
+      </c>
+      <c r="F31" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F31/100)*(1-('Sheet1 (2)'!F31/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1217%</v>
+      </c>
+      <c r="G31" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G31/100)*(1-('Sheet1 (2)'!G31/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1374%</v>
+      </c>
+      <c r="H31" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H31/100)*(1-('Sheet1 (2)'!H31/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1378%</v>
+      </c>
+      <c r="I31" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I31/100)*(1-('Sheet1 (2)'!I31/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1508%</v>
+      </c>
+      <c r="J31" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J31/100)*(1-('Sheet1 (2)'!J31/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1530%</v>
+      </c>
+      <c r="K31" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K31/100)*(1-('Sheet1 (2)'!K31/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1623%</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B32/100)*(1-('Sheet1 (2)'!B32/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2155%</v>
+      </c>
+      <c r="C32" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C32/100)*(1-('Sheet1 (2)'!C32/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1427%</v>
+      </c>
+      <c r="D32" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D32/100)*(1-('Sheet1 (2)'!D32/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1309%</v>
+      </c>
+      <c r="E32" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E32/100)*(1-('Sheet1 (2)'!E32/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1283%</v>
+      </c>
+      <c r="F32" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F32/100)*(1-('Sheet1 (2)'!F32/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1315%</v>
+      </c>
+      <c r="G32" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G32/100)*(1-('Sheet1 (2)'!G32/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1309%</v>
+      </c>
+      <c r="H32" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H32/100)*(1-('Sheet1 (2)'!H32/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1376%</v>
+      </c>
+      <c r="I32" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I32/100)*(1-('Sheet1 (2)'!I32/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1520%</v>
+      </c>
+      <c r="J32" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J32/100)*(1-('Sheet1 (2)'!J32/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1524%</v>
+      </c>
+      <c r="K32" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K32/100)*(1-('Sheet1 (2)'!K32/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1581%</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B33/100)*(1-('Sheet1 (2)'!B33/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2080%</v>
+      </c>
+      <c r="C33" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C33/100)*(1-('Sheet1 (2)'!C33/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1408%</v>
+      </c>
+      <c r="D33" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D33/100)*(1-('Sheet1 (2)'!D33/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1215%</v>
+      </c>
+      <c r="E33" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E33/100)*(1-('Sheet1 (2)'!E33/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1199%</v>
+      </c>
+      <c r="F33" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F33/100)*(1-('Sheet1 (2)'!F33/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1259%</v>
+      </c>
+      <c r="G33" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G33/100)*(1-('Sheet1 (2)'!G33/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1297%</v>
+      </c>
+      <c r="H33" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H33/100)*(1-('Sheet1 (2)'!H33/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1304%</v>
+      </c>
+      <c r="I33" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I33/100)*(1-('Sheet1 (2)'!I33/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1469%</v>
+      </c>
+      <c r="J33" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J33/100)*(1-('Sheet1 (2)'!J33/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1590%</v>
+      </c>
+      <c r="K33" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K33/100)*(1-('Sheet1 (2)'!K33/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1605%</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B34/100)*(1-('Sheet1 (2)'!B34/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2051%</v>
+      </c>
+      <c r="C34" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C34/100)*(1-('Sheet1 (2)'!C34/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1429%</v>
+      </c>
+      <c r="D34" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D34/100)*(1-('Sheet1 (2)'!D34/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1283%</v>
+      </c>
+      <c r="E34" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E34/100)*(1-('Sheet1 (2)'!E34/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1174%</v>
+      </c>
+      <c r="F34" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F34/100)*(1-('Sheet1 (2)'!F34/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1264%</v>
+      </c>
+      <c r="G34" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G34/100)*(1-('Sheet1 (2)'!G34/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1393%</v>
+      </c>
+      <c r="H34" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H34/100)*(1-('Sheet1 (2)'!H34/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1365%</v>
+      </c>
+      <c r="I34" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I34/100)*(1-('Sheet1 (2)'!I34/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1367%</v>
+      </c>
+      <c r="J34" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J34/100)*(1-('Sheet1 (2)'!J34/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1473%</v>
+      </c>
+      <c r="K34" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K34/100)*(1-('Sheet1 (2)'!K34/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1522%</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B35/100)*(1-('Sheet1 (2)'!B35/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2063%</v>
+      </c>
+      <c r="C35" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C35/100)*(1-('Sheet1 (2)'!C35/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1356%</v>
+      </c>
+      <c r="D35" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D35/100)*(1-('Sheet1 (2)'!D35/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1309%</v>
+      </c>
+      <c r="E35" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E35/100)*(1-('Sheet1 (2)'!E35/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1237%</v>
+      </c>
+      <c r="F35" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F35/100)*(1-('Sheet1 (2)'!F35/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1285%</v>
+      </c>
+      <c r="G35" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G35/100)*(1-('Sheet1 (2)'!G35/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1331%</v>
+      </c>
+      <c r="H35" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H35/100)*(1-('Sheet1 (2)'!H35/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1427%</v>
+      </c>
+      <c r="I35" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I35/100)*(1-('Sheet1 (2)'!I35/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1436%</v>
+      </c>
+      <c r="J35" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J35/100)*(1-('Sheet1 (2)'!J35/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1503%</v>
+      </c>
+      <c r="K35" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K35/100)*(1-('Sheet1 (2)'!K35/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1516%</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="9"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="16"/>
+      <c r="K36" s="16"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B38/100)*(1-('Sheet1 (2)'!B38/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2486%</v>
+      </c>
+      <c r="C38" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C38/100)*(1-('Sheet1 (2)'!C38/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1741%</v>
+      </c>
+      <c r="D38" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D38/100)*(1-('Sheet1 (2)'!D38/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1566%</v>
+      </c>
+      <c r="E38" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E38/100)*(1-('Sheet1 (2)'!E38/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1526%</v>
+      </c>
+      <c r="F38" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F38/100)*(1-('Sheet1 (2)'!F38/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1510%</v>
+      </c>
+      <c r="G38" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G38/100)*(1-('Sheet1 (2)'!G38/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1553%</v>
+      </c>
+      <c r="H38" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H38/100)*(1-('Sheet1 (2)'!H38/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1545%</v>
+      </c>
+      <c r="I38" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I38/100)*(1-('Sheet1 (2)'!I38/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1574%</v>
+      </c>
+      <c r="J38" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J38/100)*(1-('Sheet1 (2)'!J38/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1581%</v>
+      </c>
+      <c r="K38" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K38/100)*(1-('Sheet1 (2)'!K38/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1630%</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B39/100)*(1-('Sheet1 (2)'!B39/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2358%</v>
+      </c>
+      <c r="C39" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C39/100)*(1-('Sheet1 (2)'!C39/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1676%</v>
+      </c>
+      <c r="D39" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D39/100)*(1-('Sheet1 (2)'!D39/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1522%</v>
+      </c>
+      <c r="E39" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E39/100)*(1-('Sheet1 (2)'!E39/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1413%</v>
+      </c>
+      <c r="F39" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F39/100)*(1-('Sheet1 (2)'!F39/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1452%</v>
+      </c>
+      <c r="G39" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G39/100)*(1-('Sheet1 (2)'!G39/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1505%</v>
+      </c>
+      <c r="H39" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H39/100)*(1-('Sheet1 (2)'!H39/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1560%</v>
+      </c>
+      <c r="I39" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I39/100)*(1-('Sheet1 (2)'!I39/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1583%</v>
+      </c>
+      <c r="J39" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J39/100)*(1-('Sheet1 (2)'!J39/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1751%</v>
+      </c>
+      <c r="K39" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K39/100)*(1-('Sheet1 (2)'!K39/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1799%</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B40/100)*(1-('Sheet1 (2)'!B40/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2236%</v>
+      </c>
+      <c r="C40" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C40/100)*(1-('Sheet1 (2)'!C40/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1605%</v>
+      </c>
+      <c r="D40" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D40/100)*(1-('Sheet1 (2)'!D40/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1398%</v>
+      </c>
+      <c r="E40" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E40/100)*(1-('Sheet1 (2)'!E40/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1358%</v>
+      </c>
+      <c r="F40" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F40/100)*(1-('Sheet1 (2)'!F40/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1421%</v>
+      </c>
+      <c r="G40" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G40/100)*(1-('Sheet1 (2)'!G40/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1444%</v>
+      </c>
+      <c r="H40" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H40/100)*(1-('Sheet1 (2)'!H40/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1491%</v>
+      </c>
+      <c r="I40" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I40/100)*(1-('Sheet1 (2)'!I40/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1516%</v>
+      </c>
+      <c r="J40" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J40/100)*(1-('Sheet1 (2)'!J40/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1575%</v>
+      </c>
+      <c r="K40" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K40/100)*(1-('Sheet1 (2)'!K40/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1714%</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B41/100)*(1-('Sheet1 (2)'!B41/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2224%</v>
+      </c>
+      <c r="C41" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C41/100)*(1-('Sheet1 (2)'!C41/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1493%</v>
+      </c>
+      <c r="D41" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D41/100)*(1-('Sheet1 (2)'!D41/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1406%</v>
+      </c>
+      <c r="E41" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E41/100)*(1-('Sheet1 (2)'!E41/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1343%</v>
+      </c>
+      <c r="F41" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F41/100)*(1-('Sheet1 (2)'!F41/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1338%</v>
+      </c>
+      <c r="G41" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G41/100)*(1-('Sheet1 (2)'!G41/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1419%</v>
+      </c>
+      <c r="H41" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H41/100)*(1-('Sheet1 (2)'!H41/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1450%</v>
+      </c>
+      <c r="I41" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I41/100)*(1-('Sheet1 (2)'!I41/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1524%</v>
+      </c>
+      <c r="J41" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J41/100)*(1-('Sheet1 (2)'!J41/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1688%</v>
+      </c>
+      <c r="K41" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K41/100)*(1-('Sheet1 (2)'!K41/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1843%</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B42/100)*(1-('Sheet1 (2)'!B42/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2153%</v>
+      </c>
+      <c r="C42" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C42/100)*(1-('Sheet1 (2)'!C42/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1462%</v>
+      </c>
+      <c r="D42" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D42/100)*(1-('Sheet1 (2)'!D42/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1325%</v>
+      </c>
+      <c r="E42" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E42/100)*(1-('Sheet1 (2)'!E42/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1338%</v>
+      </c>
+      <c r="F42" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F42/100)*(1-('Sheet1 (2)'!F42/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1329%</v>
+      </c>
+      <c r="G42" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G42/100)*(1-('Sheet1 (2)'!G42/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1393%</v>
+      </c>
+      <c r="H42" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H42/100)*(1-('Sheet1 (2)'!H42/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1442%</v>
+      </c>
+      <c r="I42" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I42/100)*(1-('Sheet1 (2)'!I42/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1510%</v>
+      </c>
+      <c r="J42" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J42/100)*(1-('Sheet1 (2)'!J42/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1600%</v>
+      </c>
+      <c r="K42" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K42/100)*(1-('Sheet1 (2)'!K42/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1732%</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B43" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B43/100)*(1-('Sheet1 (2)'!B43/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2122%</v>
+      </c>
+      <c r="C43" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C43/100)*(1-('Sheet1 (2)'!C43/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1427%</v>
+      </c>
+      <c r="D43" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D43/100)*(1-('Sheet1 (2)'!D43/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1257%</v>
+      </c>
+      <c r="E43" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E43/100)*(1-('Sheet1 (2)'!E43/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1239%</v>
+      </c>
+      <c r="F43" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F43/100)*(1-('Sheet1 (2)'!F43/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1197%</v>
+      </c>
+      <c r="G43" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G43/100)*(1-('Sheet1 (2)'!G43/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1349%</v>
+      </c>
+      <c r="H43" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H43/100)*(1-('Sheet1 (2)'!H43/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1369%</v>
+      </c>
+      <c r="I43" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I43/100)*(1-('Sheet1 (2)'!I43/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1528%</v>
+      </c>
+      <c r="J43" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J43/100)*(1-('Sheet1 (2)'!J43/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1520%</v>
+      </c>
+      <c r="K43" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K43/100)*(1-('Sheet1 (2)'!K43/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1612%</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B44/100)*(1-('Sheet1 (2)'!B44/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2137%</v>
+      </c>
+      <c r="C44" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C44/100)*(1-('Sheet1 (2)'!C44/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1406%</v>
+      </c>
+      <c r="D44" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D44/100)*(1-('Sheet1 (2)'!D44/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1285%</v>
+      </c>
+      <c r="E44" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E44/100)*(1-('Sheet1 (2)'!E44/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1237%</v>
+      </c>
+      <c r="F44" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F44/100)*(1-('Sheet1 (2)'!F44/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1306%</v>
+      </c>
+      <c r="G44" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G44/100)*(1-('Sheet1 (2)'!G44/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1322%</v>
+      </c>
+      <c r="H44" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H44/100)*(1-('Sheet1 (2)'!H44/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1372%</v>
+      </c>
+      <c r="I44" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I44/100)*(1-('Sheet1 (2)'!I44/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1503%</v>
+      </c>
+      <c r="J44" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J44/100)*(1-('Sheet1 (2)'!J44/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1551%</v>
+      </c>
+      <c r="K44" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K44/100)*(1-('Sheet1 (2)'!K44/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1594%</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B45" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B45/100)*(1-('Sheet1 (2)'!B45/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2101%</v>
+      </c>
+      <c r="C45" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C45/100)*(1-('Sheet1 (2)'!C45/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1380%</v>
+      </c>
+      <c r="D45" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D45/100)*(1-('Sheet1 (2)'!D45/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1215%</v>
+      </c>
+      <c r="E45" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E45/100)*(1-('Sheet1 (2)'!E45/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1232%</v>
+      </c>
+      <c r="F45" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F45/100)*(1-('Sheet1 (2)'!F45/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1254%</v>
+      </c>
+      <c r="G45" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G45/100)*(1-('Sheet1 (2)'!G45/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1306%</v>
+      </c>
+      <c r="H45" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H45/100)*(1-('Sheet1 (2)'!H45/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1288%</v>
+      </c>
+      <c r="I45" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I45/100)*(1-('Sheet1 (2)'!I45/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1477%</v>
+      </c>
+      <c r="J45" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J45/100)*(1-('Sheet1 (2)'!J45/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1566%</v>
+      </c>
+      <c r="K45" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K45/100)*(1-('Sheet1 (2)'!K45/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1620%</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B46" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B46/100)*(1-('Sheet1 (2)'!B46/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2031%</v>
+      </c>
+      <c r="C46" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C46/100)*(1-('Sheet1 (2)'!C46/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1431%</v>
+      </c>
+      <c r="D46" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D46/100)*(1-('Sheet1 (2)'!D46/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1269%</v>
+      </c>
+      <c r="E46" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E46/100)*(1-('Sheet1 (2)'!E46/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1197%</v>
+      </c>
+      <c r="F46" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F46/100)*(1-('Sheet1 (2)'!F46/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1225%</v>
+      </c>
+      <c r="G46" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G46/100)*(1-('Sheet1 (2)'!G46/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1361%</v>
+      </c>
+      <c r="H46" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H46/100)*(1-('Sheet1 (2)'!H46/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1338%</v>
+      </c>
+      <c r="I46" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I46/100)*(1-('Sheet1 (2)'!I46/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1361%</v>
+      </c>
+      <c r="J46" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J46/100)*(1-('Sheet1 (2)'!J46/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1448%</v>
+      </c>
+      <c r="K46" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K46/100)*(1-('Sheet1 (2)'!K46/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1516%</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B47/100)*(1-('Sheet1 (2)'!B47/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2027%</v>
+      </c>
+      <c r="C47" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C47/100)*(1-('Sheet1 (2)'!C47/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1365%</v>
+      </c>
+      <c r="D47" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D47/100)*(1-('Sheet1 (2)'!D47/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1273%</v>
+      </c>
+      <c r="E47" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E47/100)*(1-('Sheet1 (2)'!E47/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1225%</v>
+      </c>
+      <c r="F47" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F47/100)*(1-('Sheet1 (2)'!F47/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1285%</v>
+      </c>
+      <c r="G47" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G47/100)*(1-('Sheet1 (2)'!G47/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1352%</v>
+      </c>
+      <c r="H47" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H47/100)*(1-('Sheet1 (2)'!H47/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1427%</v>
+      </c>
+      <c r="I47" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I47/100)*(1-('Sheet1 (2)'!I47/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1398%</v>
+      </c>
+      <c r="J47" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J47/100)*(1-('Sheet1 (2)'!J47/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1479%</v>
+      </c>
+      <c r="K47" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K47/100)*(1-('Sheet1 (2)'!K47/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1530%</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="9"/>
+      <c r="B48" s="16"/>
+      <c r="C48" s="16"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="16"/>
+      <c r="H48" s="16"/>
+      <c r="I48" s="16"/>
+      <c r="J48" s="16"/>
+      <c r="K48" s="16"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J49" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K49" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B50" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B50/100)*(1-('Sheet1 (2)'!B50/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2485%</v>
+      </c>
+      <c r="C50" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C50/100)*(1-('Sheet1 (2)'!C50/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1741%</v>
+      </c>
+      <c r="D50" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D50/100)*(1-('Sheet1 (2)'!D50/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1553%</v>
+      </c>
+      <c r="E50" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E50/100)*(1-('Sheet1 (2)'!E50/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1524%</v>
+      </c>
+      <c r="F50" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F50/100)*(1-('Sheet1 (2)'!F50/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1497%</v>
+      </c>
+      <c r="G50" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G50/100)*(1-('Sheet1 (2)'!G50/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1549%</v>
+      </c>
+      <c r="H50" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H50/100)*(1-('Sheet1 (2)'!H50/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1541%</v>
+      </c>
+      <c r="I50" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I50/100)*(1-('Sheet1 (2)'!I50/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1566%</v>
+      </c>
+      <c r="J50" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J50/100)*(1-('Sheet1 (2)'!J50/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1585%</v>
+      </c>
+      <c r="K50" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K50/100)*(1-('Sheet1 (2)'!K50/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1621%</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B51" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B51/100)*(1-('Sheet1 (2)'!B51/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2367%</v>
+      </c>
+      <c r="C51" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C51/100)*(1-('Sheet1 (2)'!C51/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1671%</v>
+      </c>
+      <c r="D51" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D51/100)*(1-('Sheet1 (2)'!D51/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1520%</v>
+      </c>
+      <c r="E51" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E51/100)*(1-('Sheet1 (2)'!E51/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1408%</v>
+      </c>
+      <c r="F51" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F51/100)*(1-('Sheet1 (2)'!F51/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1438%</v>
+      </c>
+      <c r="G51" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G51/100)*(1-('Sheet1 (2)'!G51/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1506%</v>
+      </c>
+      <c r="H51" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H51/100)*(1-('Sheet1 (2)'!H51/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1560%</v>
+      </c>
+      <c r="I51" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I51/100)*(1-('Sheet1 (2)'!I51/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1589%</v>
+      </c>
+      <c r="J51" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J51/100)*(1-('Sheet1 (2)'!J51/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1749%</v>
+      </c>
+      <c r="K51" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K51/100)*(1-('Sheet1 (2)'!K51/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1807%</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B52" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B52/100)*(1-('Sheet1 (2)'!B52/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2246%</v>
+      </c>
+      <c r="C52" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C52/100)*(1-('Sheet1 (2)'!C52/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1603%</v>
+      </c>
+      <c r="D52" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D52/100)*(1-('Sheet1 (2)'!D52/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1385%</v>
+      </c>
+      <c r="E52" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E52/100)*(1-('Sheet1 (2)'!E52/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1378%</v>
+      </c>
+      <c r="F52" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F52/100)*(1-('Sheet1 (2)'!F52/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1410%</v>
+      </c>
+      <c r="G52" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G52/100)*(1-('Sheet1 (2)'!G52/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1427%</v>
+      </c>
+      <c r="H52" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H52/100)*(1-('Sheet1 (2)'!H52/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1479%</v>
+      </c>
+      <c r="I52" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I52/100)*(1-('Sheet1 (2)'!I52/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1522%</v>
+      </c>
+      <c r="J52" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J52/100)*(1-('Sheet1 (2)'!J52/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1594%</v>
+      </c>
+      <c r="K52" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K52/100)*(1-('Sheet1 (2)'!K52/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1721%</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B53" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B53/100)*(1-('Sheet1 (2)'!B53/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2211%</v>
+      </c>
+      <c r="C53" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C53/100)*(1-('Sheet1 (2)'!C53/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1481%</v>
+      </c>
+      <c r="D53" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D53/100)*(1-('Sheet1 (2)'!D53/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1395%</v>
+      </c>
+      <c r="E53" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E53/100)*(1-('Sheet1 (2)'!E53/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1327%</v>
+      </c>
+      <c r="F53" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F53/100)*(1-('Sheet1 (2)'!F53/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1306%</v>
+      </c>
+      <c r="G53" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G53/100)*(1-('Sheet1 (2)'!G53/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1417%</v>
+      </c>
+      <c r="H53" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H53/100)*(1-('Sheet1 (2)'!H53/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1438%</v>
+      </c>
+      <c r="I53" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I53/100)*(1-('Sheet1 (2)'!I53/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1532%</v>
+      </c>
+      <c r="J53" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J53/100)*(1-('Sheet1 (2)'!J53/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1700%</v>
+      </c>
+      <c r="K53" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K53/100)*(1-('Sheet1 (2)'!K53/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1832%</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B54" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B54/100)*(1-('Sheet1 (2)'!B54/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2142%</v>
+      </c>
+      <c r="C54" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C54/100)*(1-('Sheet1 (2)'!C54/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1423%</v>
+      </c>
+      <c r="D54" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D54/100)*(1-('Sheet1 (2)'!D54/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1306%</v>
+      </c>
+      <c r="E54" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E54/100)*(1-('Sheet1 (2)'!E54/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1313%</v>
+      </c>
+      <c r="F54" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F54/100)*(1-('Sheet1 (2)'!F54/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1343%</v>
+      </c>
+      <c r="G54" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G54/100)*(1-('Sheet1 (2)'!G54/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1382%</v>
+      </c>
+      <c r="H54" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H54/100)*(1-('Sheet1 (2)'!H54/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1450%</v>
+      </c>
+      <c r="I54" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I54/100)*(1-('Sheet1 (2)'!I54/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1493%</v>
+      </c>
+      <c r="J54" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J54/100)*(1-('Sheet1 (2)'!J54/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1603%</v>
+      </c>
+      <c r="K54" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K54/100)*(1-('Sheet1 (2)'!K54/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1749%</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B55" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B55/100)*(1-('Sheet1 (2)'!B55/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2119%</v>
+      </c>
+      <c r="C55" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C55/100)*(1-('Sheet1 (2)'!C55/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1400%</v>
+      </c>
+      <c r="D55" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D55/100)*(1-('Sheet1 (2)'!D55/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1264%</v>
+      </c>
+      <c r="E55" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E55/100)*(1-('Sheet1 (2)'!E55/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1235%</v>
+      </c>
+      <c r="F55" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F55/100)*(1-('Sheet1 (2)'!F55/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1217%</v>
+      </c>
+      <c r="G55" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G55/100)*(1-('Sheet1 (2)'!G55/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1336%</v>
+      </c>
+      <c r="H55" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H55/100)*(1-('Sheet1 (2)'!H55/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1393%</v>
+      </c>
+      <c r="I55" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I55/100)*(1-('Sheet1 (2)'!I55/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1520%</v>
+      </c>
+      <c r="J55" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J55/100)*(1-('Sheet1 (2)'!J55/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1534%</v>
+      </c>
+      <c r="K55" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K55/100)*(1-('Sheet1 (2)'!K55/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1634%</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B56" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B56/100)*(1-('Sheet1 (2)'!B56/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2122%</v>
+      </c>
+      <c r="C56" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C56/100)*(1-('Sheet1 (2)'!C56/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1425%</v>
+      </c>
+      <c r="D56" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D56/100)*(1-('Sheet1 (2)'!D56/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1285%</v>
+      </c>
+      <c r="E56" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E56/100)*(1-('Sheet1 (2)'!E56/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1225%</v>
+      </c>
+      <c r="F56" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F56/100)*(1-('Sheet1 (2)'!F56/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1297%</v>
+      </c>
+      <c r="G56" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G56/100)*(1-('Sheet1 (2)'!G56/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1315%</v>
+      </c>
+      <c r="H56" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H56/100)*(1-('Sheet1 (2)'!H56/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1395%</v>
+      </c>
+      <c r="I56" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I56/100)*(1-('Sheet1 (2)'!I56/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1485%</v>
+      </c>
+      <c r="J56" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J56/100)*(1-('Sheet1 (2)'!J56/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1545%</v>
+      </c>
+      <c r="K56" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K56/100)*(1-('Sheet1 (2)'!K56/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1600%</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B57" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B57/100)*(1-('Sheet1 (2)'!B57/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2078%</v>
+      </c>
+      <c r="C57" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C57/100)*(1-('Sheet1 (2)'!C57/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1363%</v>
+      </c>
+      <c r="D57" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D57/100)*(1-('Sheet1 (2)'!D57/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1227%</v>
+      </c>
+      <c r="E57" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E57/100)*(1-('Sheet1 (2)'!E57/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1182%</v>
+      </c>
+      <c r="F57" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F57/100)*(1-('Sheet1 (2)'!F57/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1225%</v>
+      </c>
+      <c r="G57" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G57/100)*(1-('Sheet1 (2)'!G57/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1280%</v>
+      </c>
+      <c r="H57" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H57/100)*(1-('Sheet1 (2)'!H57/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1278%</v>
+      </c>
+      <c r="I57" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I57/100)*(1-('Sheet1 (2)'!I57/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1448%</v>
+      </c>
+      <c r="J57" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J57/100)*(1-('Sheet1 (2)'!J57/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1566%</v>
+      </c>
+      <c r="K57" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K57/100)*(1-('Sheet1 (2)'!K57/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1598%</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B58" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B58/100)*(1-('Sheet1 (2)'!B58/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2020%</v>
+      </c>
+      <c r="C58" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C58/100)*(1-('Sheet1 (2)'!C58/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1404%</v>
+      </c>
+      <c r="D58" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D58/100)*(1-('Sheet1 (2)'!D58/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1252%</v>
+      </c>
+      <c r="E58" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E58/100)*(1-('Sheet1 (2)'!E58/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1182%</v>
+      </c>
+      <c r="F58" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F58/100)*(1-('Sheet1 (2)'!F58/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1227%</v>
+      </c>
+      <c r="G58" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G58/100)*(1-('Sheet1 (2)'!G58/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1365%</v>
+      </c>
+      <c r="H58" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H58/100)*(1-('Sheet1 (2)'!H58/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1327%</v>
+      </c>
+      <c r="I58" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I58/100)*(1-('Sheet1 (2)'!I58/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1395%</v>
+      </c>
+      <c r="J58" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J58/100)*(1-('Sheet1 (2)'!J58/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1448%</v>
+      </c>
+      <c r="K58" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K58/100)*(1-('Sheet1 (2)'!K58/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1522%</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B59" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!B59/100)*(1-('Sheet1 (2)'!B59/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.2021%</v>
+      </c>
+      <c r="C59" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!C59/100)*(1-('Sheet1 (2)'!C59/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1365%</v>
+      </c>
+      <c r="D59" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!D59/100)*(1-('Sheet1 (2)'!D59/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1254%</v>
+      </c>
+      <c r="E59" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!E59/100)*(1-('Sheet1 (2)'!E59/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1220%</v>
+      </c>
+      <c r="F59" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!F59/100)*(1-('Sheet1 (2)'!F59/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1290%</v>
+      </c>
+      <c r="G59" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!G59/100)*(1-('Sheet1 (2)'!G59/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1349%</v>
+      </c>
+      <c r="H59" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!H59/100)*(1-('Sheet1 (2)'!H59/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1404%</v>
+      </c>
+      <c r="I59" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!I59/100)*(1-('Sheet1 (2)'!I59/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1382%</v>
+      </c>
+      <c r="J59" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!J59/100)*(1-('Sheet1 (2)'!J59/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1485%</v>
+      </c>
+      <c r="K59" s="6" t="str">
+        <f>"±"&amp;TEXT(100*(1.96*SQRT(('Sheet1 (2)'!K59/100)*(1-('Sheet1 (2)'!K59/100))/60000)),"0.0000")&amp;"%"</f>
+        <v>±0.1549%</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>